<commit_message>
Updated data element group to mer23 OuKFZzVk6gr
</commit_message>
<xml_diff>
--- a/data-raw/snu_x_im_distribution_configuration/23Tto24TMap.xlsx
+++ b/data-raw/snu_x_im_distribution_configuration/23Tto24TMap.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2" conformance="strict">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10215"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10808"/>
   <workbookPr dateCompatibility="0" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/faustolopezbao/Documents/GitHub/data-pack-commons/data-raw/snu_x_im_distribution_configuration/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jordanbales/Documents/Repos/data-pack-commons/data-raw/snu_x_im_distribution_configuration/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{96558AAA-0809-844B-BF97-4E765785DE11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{858FEB55-DFF6-FC40-A3E3-5C584C808E06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="36480" yWindow="940" windowWidth="33600" windowHeight="20500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Map" sheetId="1" r:id="rId1"/>
@@ -824,9 +824,6 @@
     <t>OVC_SERV.Grad.T</t>
   </si>
   <si>
-    <t>DE_GROUP-QjkuCJf6lCs</t>
-  </si>
-  <si>
     <t>2021Oct</t>
   </si>
   <si>
@@ -870,6 +867,9 @@
   </si>
   <si>
     <t>Age/Sex/ProgramStatus;Age/Sex/ProgramStatusCaregiver</t>
+  </si>
+  <si>
+    <t>DE_GROUP-OuKFZzVk6gr</t>
   </si>
 </sst>
 </file>
@@ -1401,18 +1401,19 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="10" xfId="6" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="3" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="10" xfId="7" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="19" fillId="0" borderId="10" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="11" xfId="6" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="8" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="10" xfId="8" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1783,10 +1784,10 @@
 <worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A56" zoomScaleNormal="140" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection activeCell="A44" sqref="A44"/>
-      <selection pane="topRight" activeCell="D82" sqref="D82"/>
+      <selection pane="topRight" activeCell="B12" sqref="B12:B91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1857,7 +1858,7 @@
         <v>147</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>262</v>
+        <v>277</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>3</v>
@@ -1878,7 +1879,7 @@
         <v>122</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="J2" s="1" t="s">
         <v>2</v>
@@ -1901,7 +1902,7 @@
         <v>148</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>262</v>
+        <v>277</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>3</v>
@@ -1922,7 +1923,7 @@
         <v>122</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="J3" s="1" t="s">
         <v>2</v>
@@ -1945,7 +1946,7 @@
         <v>149</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>262</v>
+        <v>277</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>127</v>
@@ -1966,10 +1967,10 @@
         <v>109</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="K4" s="3" t="s">
         <v>55</v>
@@ -1989,7 +1990,7 @@
         <v>150</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>262</v>
+        <v>277</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>127</v>
@@ -2010,10 +2011,10 @@
         <v>109</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="K5" s="3" t="s">
         <v>55</v>
@@ -2029,11 +2030,11 @@
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="4" t="s">
         <v>151</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>262</v>
+        <v>277</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>5</v>
@@ -2054,7 +2055,7 @@
         <v>248</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="J6" s="1" t="s">
         <v>64</v>
@@ -2065,7 +2066,7 @@
       <c r="L6" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="M6" s="2" t="s">
+      <c r="M6" s="4" t="s">
         <v>2</v>
       </c>
       <c r="N6" s="1" t="s">
@@ -2077,7 +2078,7 @@
         <v>152</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>262</v>
+        <v>277</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>127</v>
@@ -2098,10 +2099,10 @@
         <v>108</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="K7" s="3" t="s">
         <v>55</v>
@@ -2121,7 +2122,7 @@
         <v>153</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>262</v>
+        <v>277</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>127</v>
@@ -2142,10 +2143,10 @@
         <v>108</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="K8" s="3" t="s">
         <v>55</v>
@@ -2161,11 +2162,11 @@
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A9" s="2" t="s">
+      <c r="A9" s="4" t="s">
         <v>154</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>262</v>
+        <v>277</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>5</v>
@@ -2186,7 +2187,7 @@
         <v>249</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="J9" s="1" t="s">
         <v>64</v>
@@ -2197,7 +2198,7 @@
       <c r="L9" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="M9" s="2" t="s">
+      <c r="M9" s="4" t="s">
         <v>2</v>
       </c>
       <c r="N9" s="1" t="s">
@@ -2209,7 +2210,7 @@
         <v>155</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>262</v>
+        <v>277</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>6</v>
@@ -2230,7 +2231,7 @@
         <v>104</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="J10" s="1" t="s">
         <v>54</v>
@@ -2253,7 +2254,7 @@
         <v>156</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>262</v>
+        <v>277</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>7</v>
@@ -2274,7 +2275,7 @@
         <v>107</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="J11" s="1" t="s">
         <v>56</v>
@@ -2297,7 +2298,7 @@
         <v>157</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>262</v>
+        <v>277</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>7</v>
@@ -2318,7 +2319,7 @@
         <v>107</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="J12" s="1" t="s">
         <v>56</v>
@@ -2341,7 +2342,7 @@
         <v>158</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>262</v>
+        <v>277</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>5</v>
@@ -2362,7 +2363,7 @@
         <v>250</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="J13" s="1" t="s">
         <v>64</v>
@@ -2373,7 +2374,7 @@
       <c r="L13" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="M13" s="2" t="s">
+      <c r="M13" s="4" t="s">
         <v>2</v>
       </c>
       <c r="N13" s="1" t="s">
@@ -2385,7 +2386,7 @@
         <v>159</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>262</v>
+        <v>277</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>7</v>
@@ -2406,7 +2407,7 @@
         <v>110</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="J14" s="1" t="s">
         <v>56</v>
@@ -2429,7 +2430,7 @@
         <v>160</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>262</v>
+        <v>277</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>7</v>
@@ -2450,7 +2451,7 @@
         <v>110</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="J15" s="1" t="s">
         <v>56</v>
@@ -2469,11 +2470,11 @@
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A16" s="2" t="s">
+      <c r="A16" s="4" t="s">
         <v>161</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>262</v>
+        <v>277</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>5</v>
@@ -2494,7 +2495,7 @@
         <v>251</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="J16" s="1" t="s">
         <v>64</v>
@@ -2505,7 +2506,7 @@
       <c r="L16" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="M16" s="2" t="s">
+      <c r="M16" s="4" t="s">
         <v>2</v>
       </c>
       <c r="N16" s="1" t="s">
@@ -2517,7 +2518,7 @@
         <v>162</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>262</v>
+        <v>277</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>7</v>
@@ -2538,7 +2539,7 @@
         <v>114</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="J17" s="1" t="s">
         <v>57</v>
@@ -2561,7 +2562,7 @@
         <v>163</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>262</v>
+        <v>277</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>7</v>
@@ -2582,7 +2583,7 @@
         <v>114</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="J18" s="1" t="s">
         <v>57</v>
@@ -2605,7 +2606,7 @@
         <v>164</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>262</v>
+        <v>277</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>7</v>
@@ -2626,7 +2627,7 @@
         <v>123</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="J19" s="1" t="s">
         <v>56</v>
@@ -2649,7 +2650,7 @@
         <v>165</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>262</v>
+        <v>277</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>7</v>
@@ -2670,7 +2671,7 @@
         <v>123</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="J20" s="1" t="s">
         <v>56</v>
@@ -2689,11 +2690,11 @@
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A21" s="2" t="s">
+      <c r="A21" s="4" t="s">
         <v>166</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>262</v>
+        <v>277</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>5</v>
@@ -2714,7 +2715,7 @@
         <v>252</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="J21" s="1" t="s">
         <v>64</v>
@@ -2725,7 +2726,7 @@
       <c r="L21" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="M21" s="2" t="s">
+      <c r="M21" s="4" t="s">
         <v>2</v>
       </c>
       <c r="N21" s="1" t="s">
@@ -2737,7 +2738,7 @@
         <v>167</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>262</v>
+        <v>277</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>7</v>
@@ -2758,7 +2759,7 @@
         <v>116</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="J22" s="1" t="s">
         <v>56</v>
@@ -2781,7 +2782,7 @@
         <v>168</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>262</v>
+        <v>277</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>7</v>
@@ -2802,7 +2803,7 @@
         <v>116</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="J23" s="1" t="s">
         <v>56</v>
@@ -2825,7 +2826,7 @@
         <v>169</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>262</v>
+        <v>277</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>5</v>
@@ -2846,7 +2847,7 @@
         <v>253</v>
       </c>
       <c r="I24" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="J24" s="1" t="s">
         <v>64</v>
@@ -2857,7 +2858,7 @@
       <c r="L24" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="M24" s="2" t="s">
+      <c r="M24" s="4" t="s">
         <v>2</v>
       </c>
       <c r="N24" s="1" t="s">
@@ -2869,7 +2870,7 @@
         <v>170</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>262</v>
+        <v>277</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>7</v>
@@ -2890,7 +2891,7 @@
         <v>117</v>
       </c>
       <c r="I25" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="J25" s="1" t="s">
         <v>56</v>
@@ -2913,7 +2914,7 @@
         <v>171</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>262</v>
+        <v>277</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>7</v>
@@ -2934,7 +2935,7 @@
         <v>117</v>
       </c>
       <c r="I26" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="J26" s="1" t="s">
         <v>56</v>
@@ -2953,11 +2954,11 @@
       </c>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A27" s="2" t="s">
+      <c r="A27" s="4" t="s">
         <v>172</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>262</v>
+        <v>277</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>5</v>
@@ -2978,7 +2979,7 @@
         <v>254</v>
       </c>
       <c r="I27" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="J27" s="1" t="s">
         <v>64</v>
@@ -2989,7 +2990,7 @@
       <c r="L27" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="M27" s="2" t="s">
+      <c r="M27" s="4" t="s">
         <v>2</v>
       </c>
       <c r="N27" s="1" t="s">
@@ -3001,7 +3002,7 @@
         <v>173</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>262</v>
+        <v>277</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>7</v>
@@ -3022,7 +3023,7 @@
         <v>118</v>
       </c>
       <c r="I28" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="J28" s="1" t="s">
         <v>57</v>
@@ -3045,7 +3046,7 @@
         <v>174</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>262</v>
+        <v>277</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>7</v>
@@ -3066,7 +3067,7 @@
         <v>118</v>
       </c>
       <c r="I29" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="J29" s="1" t="s">
         <v>57</v>
@@ -3089,7 +3090,7 @@
         <v>175</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>262</v>
+        <v>277</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>7</v>
@@ -3110,10 +3111,10 @@
         <v>145</v>
       </c>
       <c r="I30" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="J30" s="1" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="K30" s="3" t="s">
         <v>63</v>
@@ -3133,7 +3134,7 @@
         <v>176</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>262</v>
+        <v>277</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>7</v>
@@ -3154,10 +3155,10 @@
         <v>145</v>
       </c>
       <c r="I31" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="J31" s="1" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="K31" s="3" t="s">
         <v>63</v>
@@ -3173,11 +3174,11 @@
       </c>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A32" s="2" t="s">
+      <c r="A32" s="4" t="s">
         <v>177</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>262</v>
+        <v>277</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>5</v>
@@ -3198,7 +3199,7 @@
         <v>255</v>
       </c>
       <c r="I32" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="J32" s="1" t="s">
         <v>64</v>
@@ -3209,7 +3210,7 @@
       <c r="L32" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="M32" s="2" t="s">
+      <c r="M32" s="4" t="s">
         <v>2</v>
       </c>
       <c r="N32" s="1" t="s">
@@ -3221,7 +3222,7 @@
         <v>178</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>262</v>
+        <v>277</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>7</v>
@@ -3242,7 +3243,7 @@
         <v>120</v>
       </c>
       <c r="I33" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="J33" s="1" t="s">
         <v>56</v>
@@ -3265,7 +3266,7 @@
         <v>179</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>262</v>
+        <v>277</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>7</v>
@@ -3286,7 +3287,7 @@
         <v>120</v>
       </c>
       <c r="I34" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="J34" s="1" t="s">
         <v>56</v>
@@ -3305,11 +3306,11 @@
       </c>
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A35" s="2" t="s">
+      <c r="A35" s="4" t="s">
         <v>180</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>262</v>
+        <v>277</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>5</v>
@@ -3330,7 +3331,7 @@
         <v>256</v>
       </c>
       <c r="I35" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="J35" s="1" t="s">
         <v>64</v>
@@ -3341,7 +3342,7 @@
       <c r="L35" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="M35" s="2" t="s">
+      <c r="M35" s="4" t="s">
         <v>2</v>
       </c>
       <c r="N35" s="1" t="s">
@@ -3353,7 +3354,7 @@
         <v>181</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>262</v>
+        <v>277</v>
       </c>
       <c r="C36" s="1" t="s">
         <v>7</v>
@@ -3374,7 +3375,7 @@
         <v>121</v>
       </c>
       <c r="I36" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="J36" s="1" t="s">
         <v>56</v>
@@ -3397,7 +3398,7 @@
         <v>182</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>262</v>
+        <v>277</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>7</v>
@@ -3418,7 +3419,7 @@
         <v>121</v>
       </c>
       <c r="I37" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="J37" s="1" t="s">
         <v>56</v>
@@ -3441,7 +3442,7 @@
         <v>183</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>262</v>
+        <v>277</v>
       </c>
       <c r="C38" s="1" t="s">
         <v>5</v>
@@ -3462,7 +3463,7 @@
         <v>257</v>
       </c>
       <c r="I38" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="J38" s="1" t="s">
         <v>64</v>
@@ -3473,7 +3474,7 @@
       <c r="L38" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="M38" s="2" t="s">
+      <c r="M38" s="4" t="s">
         <v>2</v>
       </c>
       <c r="N38" s="1" t="s">
@@ -3485,7 +3486,7 @@
         <v>184</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>262</v>
+        <v>277</v>
       </c>
       <c r="C39" s="1" t="s">
         <v>7</v>
@@ -3506,7 +3507,7 @@
         <v>113</v>
       </c>
       <c r="I39" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="J39" s="3" t="s">
         <v>2</v>
@@ -3529,7 +3530,7 @@
         <v>185</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>262</v>
+        <v>277</v>
       </c>
       <c r="C40" s="1" t="s">
         <v>7</v>
@@ -3550,7 +3551,7 @@
         <v>113</v>
       </c>
       <c r="I40" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="J40" s="3" t="s">
         <v>2</v>
@@ -3569,11 +3570,11 @@
       </c>
     </row>
     <row r="41" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A41" s="2" t="s">
+      <c r="A41" s="4" t="s">
         <v>186</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>262</v>
+        <v>277</v>
       </c>
       <c r="C41" s="2" t="s">
         <v>6</v>
@@ -3594,7 +3595,7 @@
         <v>111</v>
       </c>
       <c r="I41" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="J41" s="3" t="s">
         <v>2</v>
@@ -3617,7 +3618,7 @@
         <v>187</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>262</v>
+        <v>277</v>
       </c>
       <c r="C42" s="1" t="s">
         <v>5</v>
@@ -3638,7 +3639,7 @@
         <v>112</v>
       </c>
       <c r="I42" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="J42" s="3" t="s">
         <v>2</v>
@@ -3649,7 +3650,7 @@
       <c r="L42" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="M42" s="2" t="s">
+      <c r="M42" s="4" t="s">
         <v>2</v>
       </c>
       <c r="N42" s="1" t="s">
@@ -3661,7 +3662,7 @@
         <v>188</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>262</v>
+        <v>277</v>
       </c>
       <c r="C43" s="1" t="s">
         <v>9</v>
@@ -3682,7 +3683,7 @@
         <v>119</v>
       </c>
       <c r="I43" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="J43" s="1" t="s">
         <v>2</v>
@@ -3705,7 +3706,7 @@
         <v>189</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>262</v>
+        <v>277</v>
       </c>
       <c r="C44" s="1" t="s">
         <v>11</v>
@@ -3726,7 +3727,7 @@
         <v>111</v>
       </c>
       <c r="I44" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="J44" s="3" t="s">
         <v>2</v>
@@ -3749,7 +3750,7 @@
         <v>190</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>262</v>
+        <v>277</v>
       </c>
       <c r="C45" s="1" t="s">
         <v>13</v>
@@ -3770,7 +3771,7 @@
         <v>115</v>
       </c>
       <c r="I45" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="J45" s="1" t="s">
         <v>2</v>
@@ -3793,7 +3794,7 @@
         <v>191</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>262</v>
+        <v>277</v>
       </c>
       <c r="C46" s="1" t="s">
         <v>14</v>
@@ -3807,17 +3808,17 @@
       <c r="F46" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="G46" s="4" t="s">
-        <v>277</v>
-      </c>
-      <c r="H46" s="4" t="s">
+      <c r="G46" s="5" t="s">
         <v>276</v>
       </c>
+      <c r="H46" s="5" t="s">
+        <v>275</v>
+      </c>
       <c r="I46" s="1" t="s">
-        <v>263</v>
-      </c>
-      <c r="J46" s="5" t="s">
-        <v>275</v>
+        <v>262</v>
+      </c>
+      <c r="J46" s="6" t="s">
+        <v>274</v>
       </c>
       <c r="K46" s="3" t="s">
         <v>55</v>
@@ -3837,7 +3838,7 @@
         <v>261</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>262</v>
+        <v>277</v>
       </c>
       <c r="C47" s="1" t="s">
         <v>14</v>
@@ -3851,17 +3852,17 @@
       <c r="F47" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="G47" s="4" t="s">
-        <v>277</v>
-      </c>
-      <c r="H47" s="4" t="s">
+      <c r="G47" s="5" t="s">
         <v>276</v>
       </c>
+      <c r="H47" s="5" t="s">
+        <v>275</v>
+      </c>
       <c r="I47" s="1" t="s">
-        <v>263</v>
-      </c>
-      <c r="J47" s="5" t="s">
-        <v>275</v>
+        <v>262</v>
+      </c>
+      <c r="J47" s="6" t="s">
+        <v>274</v>
       </c>
       <c r="K47" s="3" t="s">
         <v>55</v>
@@ -3877,46 +3878,46 @@
       </c>
     </row>
     <row r="48" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A48" s="6" t="s">
+      <c r="A48" s="7" t="s">
         <v>258</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>262</v>
-      </c>
-      <c r="C48" s="6" t="s">
+        <v>277</v>
+      </c>
+      <c r="C48" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="D48" s="6" t="s">
+      <c r="D48" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="E48" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="F48" s="6" t="s">
+      <c r="E48" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="F48" s="7" t="s">
         <v>81</v>
       </c>
       <c r="G48" s="2" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="H48" s="2" t="s">
-        <v>271</v>
-      </c>
-      <c r="I48" s="6" t="s">
-        <v>263</v>
-      </c>
-      <c r="J48" s="7" t="s">
+        <v>270</v>
+      </c>
+      <c r="I48" s="7" t="s">
+        <v>262</v>
+      </c>
+      <c r="J48" s="8" t="s">
         <v>259</v>
       </c>
-      <c r="K48" s="6" t="s">
+      <c r="K48" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="L48" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="M48" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="N48" s="6" t="s">
+      <c r="L48" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="M48" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="N48" s="7" t="s">
         <v>59</v>
       </c>
     </row>
@@ -3925,7 +3926,7 @@
         <v>192</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>262</v>
+        <v>277</v>
       </c>
       <c r="C49" s="1" t="s">
         <v>15</v>
@@ -3946,10 +3947,10 @@
         <v>132</v>
       </c>
       <c r="I49" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="J49" s="1" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="K49" s="3" t="s">
         <v>63</v>
@@ -3969,7 +3970,7 @@
         <v>193</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>262</v>
+        <v>277</v>
       </c>
       <c r="C50" s="1" t="s">
         <v>15</v>
@@ -3990,10 +3991,10 @@
         <v>132</v>
       </c>
       <c r="I50" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="J50" s="1" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="K50" s="3" t="s">
         <v>63</v>
@@ -4013,7 +4014,7 @@
         <v>194</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>262</v>
+        <v>277</v>
       </c>
       <c r="C51" s="1" t="s">
         <v>16</v>
@@ -4034,7 +4035,7 @@
         <v>103</v>
       </c>
       <c r="I51" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="J51" s="1" t="s">
         <v>61</v>
@@ -4057,7 +4058,7 @@
         <v>195</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>262</v>
+        <v>277</v>
       </c>
       <c r="C52" s="1" t="s">
         <v>16</v>
@@ -4078,7 +4079,7 @@
         <v>103</v>
       </c>
       <c r="I52" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="J52" s="1" t="s">
         <v>62</v>
@@ -4101,7 +4102,7 @@
         <v>196</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>262</v>
+        <v>277</v>
       </c>
       <c r="C53" s="1" t="s">
         <v>18</v>
@@ -4122,10 +4123,10 @@
         <v>104</v>
       </c>
       <c r="I53" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="J53" s="1" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="K53" s="3" t="s">
         <v>63</v>
@@ -4145,7 +4146,7 @@
         <v>197</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>262</v>
+        <v>277</v>
       </c>
       <c r="C54" s="1" t="s">
         <v>18</v>
@@ -4166,10 +4167,10 @@
         <v>106</v>
       </c>
       <c r="I54" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="J54" s="1" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="K54" s="3" t="s">
         <v>63</v>
@@ -4189,7 +4190,7 @@
         <v>198</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>262</v>
+        <v>277</v>
       </c>
       <c r="C55" s="1" t="s">
         <v>18</v>
@@ -4210,10 +4211,10 @@
         <v>106</v>
       </c>
       <c r="I55" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="J55" s="1" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="K55" s="3" t="s">
         <v>63</v>
@@ -4233,7 +4234,7 @@
         <v>199</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>262</v>
+        <v>277</v>
       </c>
       <c r="C56" s="1" t="s">
         <v>18</v>
@@ -4254,10 +4255,10 @@
         <v>106</v>
       </c>
       <c r="I56" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="J56" s="1" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="K56" s="3" t="s">
         <v>63</v>
@@ -4277,7 +4278,7 @@
         <v>260</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>262</v>
+        <v>277</v>
       </c>
       <c r="C57" s="1" t="s">
         <v>5</v>
@@ -4298,7 +4299,7 @@
         <v>233</v>
       </c>
       <c r="I57" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="J57" s="1" t="s">
         <v>64</v>
@@ -4309,7 +4310,7 @@
       <c r="L57" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="M57" s="2" t="s">
+      <c r="M57" s="4" t="s">
         <v>2</v>
       </c>
       <c r="N57" s="1" t="s">
@@ -4321,7 +4322,7 @@
         <v>200</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>262</v>
+        <v>277</v>
       </c>
       <c r="C58" s="1" t="s">
         <v>21</v>
@@ -4342,7 +4343,7 @@
         <v>104</v>
       </c>
       <c r="I58" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="J58" s="1" t="s">
         <v>54</v>
@@ -4362,10 +4363,10 @@
     </row>
     <row r="59" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>262</v>
+        <v>277</v>
       </c>
       <c r="C59" s="1" t="s">
         <v>22</v>
@@ -4386,7 +4387,7 @@
         <v>104</v>
       </c>
       <c r="I59" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="J59" s="1" t="s">
         <v>64</v>
@@ -4406,10 +4407,10 @@
     </row>
     <row r="60" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>262</v>
+        <v>277</v>
       </c>
       <c r="C60" s="1" t="s">
         <v>22</v>
@@ -4430,7 +4431,7 @@
         <v>111</v>
       </c>
       <c r="I60" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="J60" s="3" t="s">
         <v>2</v>
@@ -4453,7 +4454,7 @@
         <v>201</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>262</v>
+        <v>277</v>
       </c>
       <c r="C61" s="1" t="s">
         <v>23</v>
@@ -4474,7 +4475,7 @@
         <v>104</v>
       </c>
       <c r="I61" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="J61" s="1" t="s">
         <v>64</v>
@@ -4497,7 +4498,7 @@
         <v>202</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>262</v>
+        <v>277</v>
       </c>
       <c r="C62" s="1" t="s">
         <v>23</v>
@@ -4518,7 +4519,7 @@
         <v>111</v>
       </c>
       <c r="I62" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="J62" s="3" t="s">
         <v>2</v>
@@ -4541,7 +4542,7 @@
         <v>203</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>262</v>
+        <v>277</v>
       </c>
       <c r="C63" s="1" t="s">
         <v>24</v>
@@ -4562,10 +4563,10 @@
         <v>132</v>
       </c>
       <c r="I63" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="J63" s="1" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="K63" s="3" t="s">
         <v>55</v>
@@ -4585,7 +4586,7 @@
         <v>204</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>262</v>
+        <v>277</v>
       </c>
       <c r="C64" s="1" t="s">
         <v>24</v>
@@ -4606,10 +4607,10 @@
         <v>132</v>
       </c>
       <c r="I64" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="J64" s="1" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="K64" s="3" t="s">
         <v>55</v>
@@ -4629,7 +4630,7 @@
         <v>205</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>262</v>
+        <v>277</v>
       </c>
       <c r="C65" s="1" t="s">
         <v>25</v>
@@ -4650,7 +4651,7 @@
         <v>132</v>
       </c>
       <c r="I65" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="J65" s="1" t="s">
         <v>126</v>
@@ -4673,7 +4674,7 @@
         <v>206</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>262</v>
+        <v>277</v>
       </c>
       <c r="C66" s="1" t="s">
         <v>25</v>
@@ -4694,7 +4695,7 @@
         <v>132</v>
       </c>
       <c r="I66" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="J66" s="1" t="s">
         <v>126</v>
@@ -4717,7 +4718,7 @@
         <v>207</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>262</v>
+        <v>277</v>
       </c>
       <c r="C67" s="1" t="s">
         <v>25</v>
@@ -4738,7 +4739,7 @@
         <v>132</v>
       </c>
       <c r="I67" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="J67" s="1" t="s">
         <v>126</v>
@@ -4761,7 +4762,7 @@
         <v>208</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>262</v>
+        <v>277</v>
       </c>
       <c r="C68" s="1" t="s">
         <v>25</v>
@@ -4782,7 +4783,7 @@
         <v>132</v>
       </c>
       <c r="I68" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="J68" s="1" t="s">
         <v>126</v>
@@ -4805,7 +4806,7 @@
         <v>209</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>262</v>
+        <v>277</v>
       </c>
       <c r="C69" s="1" t="s">
         <v>26</v>
@@ -4826,10 +4827,10 @@
         <v>104</v>
       </c>
       <c r="I69" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="J69" s="1" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="K69" s="3" t="s">
         <v>55</v>
@@ -4849,7 +4850,7 @@
         <v>210</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>262</v>
+        <v>277</v>
       </c>
       <c r="C70" s="1" t="s">
         <v>26</v>
@@ -4870,10 +4871,10 @@
         <v>106</v>
       </c>
       <c r="I70" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="J70" s="1" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="K70" s="3" t="s">
         <v>55</v>
@@ -4893,7 +4894,7 @@
         <v>211</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>262</v>
+        <v>277</v>
       </c>
       <c r="C71" s="1" t="s">
         <v>26</v>
@@ -4914,10 +4915,10 @@
         <v>106</v>
       </c>
       <c r="I71" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="J71" s="1" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="K71" s="3" t="s">
         <v>55</v>
@@ -4937,7 +4938,7 @@
         <v>212</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>262</v>
+        <v>277</v>
       </c>
       <c r="C72" s="1" t="s">
         <v>26</v>
@@ -4958,10 +4959,10 @@
         <v>106</v>
       </c>
       <c r="I72" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="J72" s="1" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="K72" s="3" t="s">
         <v>55</v>
@@ -4977,11 +4978,11 @@
       </c>
     </row>
     <row r="73" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A73" s="2" t="s">
+      <c r="A73" s="4" t="s">
         <v>213</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>262</v>
+        <v>277</v>
       </c>
       <c r="C73" s="1" t="s">
         <v>5</v>
@@ -5002,7 +5003,7 @@
         <v>235</v>
       </c>
       <c r="I73" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="J73" s="1" t="s">
         <v>64</v>
@@ -5013,7 +5014,7 @@
       <c r="L73" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="M73" s="2" t="s">
+      <c r="M73" s="4" t="s">
         <v>2</v>
       </c>
       <c r="N73" s="1" t="s">
@@ -5025,7 +5026,7 @@
         <v>214</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>262</v>
+        <v>277</v>
       </c>
       <c r="C74" s="1" t="s">
         <v>27</v>
@@ -5046,10 +5047,10 @@
         <v>105</v>
       </c>
       <c r="I74" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="J74" s="1" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="K74" s="3" t="s">
         <v>55</v>
@@ -5069,7 +5070,7 @@
         <v>215</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>262</v>
+        <v>277</v>
       </c>
       <c r="C75" s="1" t="s">
         <v>28</v>
@@ -5090,10 +5091,10 @@
         <v>105</v>
       </c>
       <c r="I75" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="J75" s="1" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="K75" s="3" t="s">
         <v>55</v>
@@ -5113,7 +5114,7 @@
         <v>216</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>262</v>
+        <v>277</v>
       </c>
       <c r="C76" s="1" t="s">
         <v>28</v>
@@ -5134,7 +5135,7 @@
         <v>112</v>
       </c>
       <c r="I76" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="J76" s="3" t="s">
         <v>2</v>
@@ -5157,7 +5158,7 @@
         <v>217</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>262</v>
+        <v>277</v>
       </c>
       <c r="C77" s="1" t="s">
         <v>27</v>
@@ -5178,7 +5179,7 @@
         <v>112</v>
       </c>
       <c r="I77" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="J77" s="3" t="s">
         <v>2</v>
@@ -5201,7 +5202,7 @@
         <v>218</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>262</v>
+        <v>277</v>
       </c>
       <c r="C78" s="2" t="s">
         <v>30</v>
@@ -5222,7 +5223,7 @@
         <v>112</v>
       </c>
       <c r="I78" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="J78" s="3" t="s">
         <v>2</v>
@@ -5245,7 +5246,7 @@
         <v>219</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>262</v>
+        <v>277</v>
       </c>
       <c r="C79" s="2" t="s">
         <v>30</v>
@@ -5266,7 +5267,7 @@
         <v>112</v>
       </c>
       <c r="I79" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="J79" s="3" t="s">
         <v>2</v>
@@ -5289,7 +5290,7 @@
         <v>220</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>262</v>
+        <v>277</v>
       </c>
       <c r="C80" s="2" t="s">
         <v>30</v>
@@ -5310,10 +5311,10 @@
         <v>134</v>
       </c>
       <c r="I80" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="J80" s="1" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="K80" s="3" t="s">
         <v>55</v>
@@ -5333,7 +5334,7 @@
         <v>221</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>262</v>
+        <v>277</v>
       </c>
       <c r="C81" s="2" t="s">
         <v>30</v>
@@ -5354,10 +5355,10 @@
         <v>134</v>
       </c>
       <c r="I81" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="J81" s="1" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="K81" s="3" t="s">
         <v>55</v>
@@ -5377,7 +5378,7 @@
         <v>222</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>262</v>
+        <v>277</v>
       </c>
       <c r="C82" s="1" t="s">
         <v>32</v>
@@ -5398,7 +5399,7 @@
         <v>138</v>
       </c>
       <c r="I82" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="J82" s="1" t="s">
         <v>126</v>
@@ -5421,7 +5422,7 @@
         <v>223</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>262</v>
+        <v>277</v>
       </c>
       <c r="C83" s="1" t="s">
         <v>32</v>
@@ -5442,7 +5443,7 @@
         <v>138</v>
       </c>
       <c r="I83" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="J83" s="1" t="s">
         <v>126</v>
@@ -5465,7 +5466,7 @@
         <v>224</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>262</v>
+        <v>277</v>
       </c>
       <c r="C84" s="1" t="s">
         <v>32</v>
@@ -5486,7 +5487,7 @@
         <v>138</v>
       </c>
       <c r="I84" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="J84" s="1" t="s">
         <v>126</v>
@@ -5509,7 +5510,7 @@
         <v>225</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>262</v>
+        <v>277</v>
       </c>
       <c r="C85" s="1" t="s">
         <v>32</v>
@@ -5530,7 +5531,7 @@
         <v>138</v>
       </c>
       <c r="I85" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="J85" s="1" t="s">
         <v>126</v>
@@ -5553,7 +5554,7 @@
         <v>226</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>262</v>
+        <v>277</v>
       </c>
       <c r="C86" s="1" t="s">
         <v>34</v>
@@ -5574,10 +5575,10 @@
         <v>105</v>
       </c>
       <c r="I86" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="J86" s="1" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="K86" s="3" t="s">
         <v>75</v>
@@ -5597,7 +5598,7 @@
         <v>227</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>262</v>
+        <v>277</v>
       </c>
       <c r="C87" s="1" t="s">
         <v>34</v>
@@ -5618,10 +5619,10 @@
         <v>105</v>
       </c>
       <c r="I87" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="J87" s="1" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="K87" s="3" t="s">
         <v>75</v>
@@ -5637,11 +5638,11 @@
       </c>
     </row>
     <row r="88" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A88" s="2" t="s">
+      <c r="A88" s="4" t="s">
         <v>228</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>262</v>
+        <v>277</v>
       </c>
       <c r="C88" s="1" t="s">
         <v>5</v>
@@ -5662,7 +5663,7 @@
         <v>237</v>
       </c>
       <c r="I88" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="J88" s="1" t="s">
         <v>64</v>
@@ -5673,7 +5674,7 @@
       <c r="L88" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="M88" s="2" t="s">
+      <c r="M88" s="4" t="s">
         <v>2</v>
       </c>
       <c r="N88" s="1" t="s">
@@ -5685,7 +5686,7 @@
         <v>229</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>262</v>
+        <v>277</v>
       </c>
       <c r="C89" s="1" t="s">
         <v>34</v>
@@ -5706,10 +5707,10 @@
         <v>105</v>
       </c>
       <c r="I89" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="J89" s="1" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="K89" s="3" t="s">
         <v>75</v>
@@ -5729,9 +5730,9 @@
         <v>230</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>262</v>
-      </c>
-      <c r="C90" s="8" t="s">
+        <v>277</v>
+      </c>
+      <c r="C90" s="9" t="s">
         <v>0</v>
       </c>
       <c r="D90" s="1" t="s">
@@ -5750,65 +5751,65 @@
         <v>105</v>
       </c>
       <c r="I90" s="1" t="s">
-        <v>263</v>
-      </c>
-      <c r="J90" s="8" t="s">
+        <v>262</v>
+      </c>
+      <c r="J90" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="K90" s="9" t="s">
+      <c r="K90" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="L90" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="M90" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="N90" s="8" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="91" spans="1:14" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A91" s="10" t="s">
-        <v>270</v>
+      <c r="L90" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="M90" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="N90" s="9" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="91" spans="1:14" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A91" s="11" t="s">
+        <v>269</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>262</v>
-      </c>
-      <c r="C91" s="12" t="s">
+        <v>277</v>
+      </c>
+      <c r="C91" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="D91" s="11" t="s">
+      <c r="D91" s="12" t="s">
         <v>88</v>
       </c>
-      <c r="E91" s="11" t="s">
+      <c r="E91" s="12" t="s">
         <v>36</v>
       </c>
       <c r="F91" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="G91" s="10" t="s">
+      <c r="G91" s="11" t="s">
+        <v>273</v>
+      </c>
+      <c r="H91" s="11" t="s">
+        <v>272</v>
+      </c>
+      <c r="I91" s="12" t="s">
+        <v>262</v>
+      </c>
+      <c r="J91" s="6" t="s">
         <v>274</v>
       </c>
-      <c r="H91" s="10" t="s">
-        <v>273</v>
-      </c>
-      <c r="I91" s="11" t="s">
-        <v>263</v>
-      </c>
-      <c r="J91" s="5" t="s">
-        <v>275</v>
-      </c>
-      <c r="K91" s="12" t="s">
+      <c r="K91" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="L91" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="M91" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="N91" s="12" t="s">
+      <c r="L91" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="M91" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="N91" s="13" t="s">
         <v>59</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated period to 2022Oct from 2021Oct
</commit_message>
<xml_diff>
--- a/data-raw/snu_x_im_distribution_configuration/23Tto24TMap.xlsx
+++ b/data-raw/snu_x_im_distribution_configuration/23Tto24TMap.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jordanbales/Documents/Repos/data-pack-commons/data-raw/snu_x_im_distribution_configuration/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{858FEB55-DFF6-FC40-A3E3-5C584C808E06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{2E10F037-3E07-5348-9701-0B7EA94D4F2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="16000" yWindow="500" windowWidth="32000" windowHeight="26160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Map" sheetId="1" r:id="rId1"/>
@@ -824,9 +824,6 @@
     <t>OVC_SERV.Grad.T</t>
   </si>
   <si>
-    <t>2021Oct</t>
-  </si>
-  <si>
     <t>PrEP_CT.T</t>
   </si>
   <si>
@@ -870,6 +867,9 @@
   </si>
   <si>
     <t>DE_GROUP-OuKFZzVk6gr</t>
+  </si>
+  <si>
+    <t>2022Oct</t>
   </si>
 </sst>
 </file>
@@ -1784,10 +1784,10 @@
 <worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N91"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="D1" activePane="topRight" state="frozen"/>
       <selection activeCell="A44" sqref="A44"/>
-      <selection pane="topRight" activeCell="B12" sqref="B12:B91"/>
+      <selection pane="topRight" activeCell="I3" sqref="I1:I1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1858,7 +1858,7 @@
         <v>147</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>3</v>
@@ -1879,7 +1879,7 @@
         <v>122</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>262</v>
+        <v>277</v>
       </c>
       <c r="J2" s="1" t="s">
         <v>2</v>
@@ -1902,7 +1902,7 @@
         <v>148</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>3</v>
@@ -1923,7 +1923,7 @@
         <v>122</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>262</v>
+        <v>277</v>
       </c>
       <c r="J3" s="1" t="s">
         <v>2</v>
@@ -1946,7 +1946,7 @@
         <v>149</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>127</v>
@@ -1967,10 +1967,10 @@
         <v>109</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>262</v>
+        <v>277</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="K4" s="3" t="s">
         <v>55</v>
@@ -1990,7 +1990,7 @@
         <v>150</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>127</v>
@@ -2011,10 +2011,10 @@
         <v>109</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>262</v>
+        <v>277</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="K5" s="3" t="s">
         <v>55</v>
@@ -2034,7 +2034,7 @@
         <v>151</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>5</v>
@@ -2055,7 +2055,7 @@
         <v>248</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>262</v>
+        <v>277</v>
       </c>
       <c r="J6" s="1" t="s">
         <v>64</v>
@@ -2078,7 +2078,7 @@
         <v>152</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>127</v>
@@ -2099,10 +2099,10 @@
         <v>108</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>262</v>
+        <v>277</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="K7" s="3" t="s">
         <v>55</v>
@@ -2122,7 +2122,7 @@
         <v>153</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>127</v>
@@ -2143,10 +2143,10 @@
         <v>108</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>262</v>
+        <v>277</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="K8" s="3" t="s">
         <v>55</v>
@@ -2166,7 +2166,7 @@
         <v>154</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>5</v>
@@ -2187,7 +2187,7 @@
         <v>249</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>262</v>
+        <v>277</v>
       </c>
       <c r="J9" s="1" t="s">
         <v>64</v>
@@ -2210,7 +2210,7 @@
         <v>155</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>6</v>
@@ -2231,7 +2231,7 @@
         <v>104</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>262</v>
+        <v>277</v>
       </c>
       <c r="J10" s="1" t="s">
         <v>54</v>
@@ -2254,7 +2254,7 @@
         <v>156</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>7</v>
@@ -2275,7 +2275,7 @@
         <v>107</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>262</v>
+        <v>277</v>
       </c>
       <c r="J11" s="1" t="s">
         <v>56</v>
@@ -2298,7 +2298,7 @@
         <v>157</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>7</v>
@@ -2319,7 +2319,7 @@
         <v>107</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>262</v>
+        <v>277</v>
       </c>
       <c r="J12" s="1" t="s">
         <v>56</v>
@@ -2342,7 +2342,7 @@
         <v>158</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>5</v>
@@ -2363,7 +2363,7 @@
         <v>250</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>262</v>
+        <v>277</v>
       </c>
       <c r="J13" s="1" t="s">
         <v>64</v>
@@ -2386,7 +2386,7 @@
         <v>159</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>7</v>
@@ -2407,7 +2407,7 @@
         <v>110</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>262</v>
+        <v>277</v>
       </c>
       <c r="J14" s="1" t="s">
         <v>56</v>
@@ -2430,7 +2430,7 @@
         <v>160</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>7</v>
@@ -2451,7 +2451,7 @@
         <v>110</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>262</v>
+        <v>277</v>
       </c>
       <c r="J15" s="1" t="s">
         <v>56</v>
@@ -2474,7 +2474,7 @@
         <v>161</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>5</v>
@@ -2495,7 +2495,7 @@
         <v>251</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>262</v>
+        <v>277</v>
       </c>
       <c r="J16" s="1" t="s">
         <v>64</v>
@@ -2518,7 +2518,7 @@
         <v>162</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>7</v>
@@ -2539,7 +2539,7 @@
         <v>114</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>262</v>
+        <v>277</v>
       </c>
       <c r="J17" s="1" t="s">
         <v>57</v>
@@ -2562,7 +2562,7 @@
         <v>163</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>7</v>
@@ -2583,7 +2583,7 @@
         <v>114</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>262</v>
+        <v>277</v>
       </c>
       <c r="J18" s="1" t="s">
         <v>57</v>
@@ -2606,7 +2606,7 @@
         <v>164</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>7</v>
@@ -2627,7 +2627,7 @@
         <v>123</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>262</v>
+        <v>277</v>
       </c>
       <c r="J19" s="1" t="s">
         <v>56</v>
@@ -2650,7 +2650,7 @@
         <v>165</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>7</v>
@@ -2671,7 +2671,7 @@
         <v>123</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>262</v>
+        <v>277</v>
       </c>
       <c r="J20" s="1" t="s">
         <v>56</v>
@@ -2694,7 +2694,7 @@
         <v>166</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>5</v>
@@ -2715,7 +2715,7 @@
         <v>252</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>262</v>
+        <v>277</v>
       </c>
       <c r="J21" s="1" t="s">
         <v>64</v>
@@ -2738,7 +2738,7 @@
         <v>167</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>7</v>
@@ -2759,7 +2759,7 @@
         <v>116</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>262</v>
+        <v>277</v>
       </c>
       <c r="J22" s="1" t="s">
         <v>56</v>
@@ -2782,7 +2782,7 @@
         <v>168</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>7</v>
@@ -2803,7 +2803,7 @@
         <v>116</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>262</v>
+        <v>277</v>
       </c>
       <c r="J23" s="1" t="s">
         <v>56</v>
@@ -2826,7 +2826,7 @@
         <v>169</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>5</v>
@@ -2847,7 +2847,7 @@
         <v>253</v>
       </c>
       <c r="I24" s="1" t="s">
-        <v>262</v>
+        <v>277</v>
       </c>
       <c r="J24" s="1" t="s">
         <v>64</v>
@@ -2870,7 +2870,7 @@
         <v>170</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>7</v>
@@ -2891,7 +2891,7 @@
         <v>117</v>
       </c>
       <c r="I25" s="1" t="s">
-        <v>262</v>
+        <v>277</v>
       </c>
       <c r="J25" s="1" t="s">
         <v>56</v>
@@ -2914,7 +2914,7 @@
         <v>171</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>7</v>
@@ -2935,7 +2935,7 @@
         <v>117</v>
       </c>
       <c r="I26" s="1" t="s">
-        <v>262</v>
+        <v>277</v>
       </c>
       <c r="J26" s="1" t="s">
         <v>56</v>
@@ -2958,7 +2958,7 @@
         <v>172</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>5</v>
@@ -2979,7 +2979,7 @@
         <v>254</v>
       </c>
       <c r="I27" s="1" t="s">
-        <v>262</v>
+        <v>277</v>
       </c>
       <c r="J27" s="1" t="s">
         <v>64</v>
@@ -3002,7 +3002,7 @@
         <v>173</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>7</v>
@@ -3023,7 +3023,7 @@
         <v>118</v>
       </c>
       <c r="I28" s="1" t="s">
-        <v>262</v>
+        <v>277</v>
       </c>
       <c r="J28" s="1" t="s">
         <v>57</v>
@@ -3046,7 +3046,7 @@
         <v>174</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>7</v>
@@ -3067,7 +3067,7 @@
         <v>118</v>
       </c>
       <c r="I29" s="1" t="s">
-        <v>262</v>
+        <v>277</v>
       </c>
       <c r="J29" s="1" t="s">
         <v>57</v>
@@ -3090,7 +3090,7 @@
         <v>175</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>7</v>
@@ -3111,10 +3111,10 @@
         <v>145</v>
       </c>
       <c r="I30" s="1" t="s">
-        <v>262</v>
+        <v>277</v>
       </c>
       <c r="J30" s="1" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="K30" s="3" t="s">
         <v>63</v>
@@ -3134,7 +3134,7 @@
         <v>176</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>7</v>
@@ -3155,10 +3155,10 @@
         <v>145</v>
       </c>
       <c r="I31" s="1" t="s">
-        <v>262</v>
+        <v>277</v>
       </c>
       <c r="J31" s="1" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="K31" s="3" t="s">
         <v>63</v>
@@ -3178,7 +3178,7 @@
         <v>177</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>5</v>
@@ -3199,7 +3199,7 @@
         <v>255</v>
       </c>
       <c r="I32" s="1" t="s">
-        <v>262</v>
+        <v>277</v>
       </c>
       <c r="J32" s="1" t="s">
         <v>64</v>
@@ -3222,7 +3222,7 @@
         <v>178</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>7</v>
@@ -3243,7 +3243,7 @@
         <v>120</v>
       </c>
       <c r="I33" s="1" t="s">
-        <v>262</v>
+        <v>277</v>
       </c>
       <c r="J33" s="1" t="s">
         <v>56</v>
@@ -3266,7 +3266,7 @@
         <v>179</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>7</v>
@@ -3287,7 +3287,7 @@
         <v>120</v>
       </c>
       <c r="I34" s="1" t="s">
-        <v>262</v>
+        <v>277</v>
       </c>
       <c r="J34" s="1" t="s">
         <v>56</v>
@@ -3310,7 +3310,7 @@
         <v>180</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>5</v>
@@ -3331,7 +3331,7 @@
         <v>256</v>
       </c>
       <c r="I35" s="1" t="s">
-        <v>262</v>
+        <v>277</v>
       </c>
       <c r="J35" s="1" t="s">
         <v>64</v>
@@ -3354,7 +3354,7 @@
         <v>181</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C36" s="1" t="s">
         <v>7</v>
@@ -3375,7 +3375,7 @@
         <v>121</v>
       </c>
       <c r="I36" s="1" t="s">
-        <v>262</v>
+        <v>277</v>
       </c>
       <c r="J36" s="1" t="s">
         <v>56</v>
@@ -3398,7 +3398,7 @@
         <v>182</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>7</v>
@@ -3419,7 +3419,7 @@
         <v>121</v>
       </c>
       <c r="I37" s="1" t="s">
-        <v>262</v>
+        <v>277</v>
       </c>
       <c r="J37" s="1" t="s">
         <v>56</v>
@@ -3442,7 +3442,7 @@
         <v>183</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C38" s="1" t="s">
         <v>5</v>
@@ -3463,7 +3463,7 @@
         <v>257</v>
       </c>
       <c r="I38" s="1" t="s">
-        <v>262</v>
+        <v>277</v>
       </c>
       <c r="J38" s="1" t="s">
         <v>64</v>
@@ -3486,7 +3486,7 @@
         <v>184</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C39" s="1" t="s">
         <v>7</v>
@@ -3507,7 +3507,7 @@
         <v>113</v>
       </c>
       <c r="I39" s="1" t="s">
-        <v>262</v>
+        <v>277</v>
       </c>
       <c r="J39" s="3" t="s">
         <v>2</v>
@@ -3530,7 +3530,7 @@
         <v>185</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C40" s="1" t="s">
         <v>7</v>
@@ -3551,7 +3551,7 @@
         <v>113</v>
       </c>
       <c r="I40" s="1" t="s">
-        <v>262</v>
+        <v>277</v>
       </c>
       <c r="J40" s="3" t="s">
         <v>2</v>
@@ -3574,7 +3574,7 @@
         <v>186</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C41" s="2" t="s">
         <v>6</v>
@@ -3595,7 +3595,7 @@
         <v>111</v>
       </c>
       <c r="I41" s="1" t="s">
-        <v>262</v>
+        <v>277</v>
       </c>
       <c r="J41" s="3" t="s">
         <v>2</v>
@@ -3618,7 +3618,7 @@
         <v>187</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C42" s="1" t="s">
         <v>5</v>
@@ -3639,7 +3639,7 @@
         <v>112</v>
       </c>
       <c r="I42" s="1" t="s">
-        <v>262</v>
+        <v>277</v>
       </c>
       <c r="J42" s="3" t="s">
         <v>2</v>
@@ -3662,7 +3662,7 @@
         <v>188</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C43" s="1" t="s">
         <v>9</v>
@@ -3683,7 +3683,7 @@
         <v>119</v>
       </c>
       <c r="I43" s="1" t="s">
-        <v>262</v>
+        <v>277</v>
       </c>
       <c r="J43" s="1" t="s">
         <v>2</v>
@@ -3706,7 +3706,7 @@
         <v>189</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C44" s="1" t="s">
         <v>11</v>
@@ -3727,7 +3727,7 @@
         <v>111</v>
       </c>
       <c r="I44" s="1" t="s">
-        <v>262</v>
+        <v>277</v>
       </c>
       <c r="J44" s="3" t="s">
         <v>2</v>
@@ -3750,7 +3750,7 @@
         <v>190</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C45" s="1" t="s">
         <v>13</v>
@@ -3771,7 +3771,7 @@
         <v>115</v>
       </c>
       <c r="I45" s="1" t="s">
-        <v>262</v>
+        <v>277</v>
       </c>
       <c r="J45" s="1" t="s">
         <v>2</v>
@@ -3794,7 +3794,7 @@
         <v>191</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C46" s="1" t="s">
         <v>14</v>
@@ -3809,16 +3809,16 @@
         <v>81</v>
       </c>
       <c r="G46" s="5" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="H46" s="5" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="I46" s="1" t="s">
-        <v>262</v>
+        <v>277</v>
       </c>
       <c r="J46" s="6" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="K46" s="3" t="s">
         <v>55</v>
@@ -3838,7 +3838,7 @@
         <v>261</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C47" s="1" t="s">
         <v>14</v>
@@ -3853,16 +3853,16 @@
         <v>81</v>
       </c>
       <c r="G47" s="5" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="H47" s="5" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="I47" s="1" t="s">
-        <v>262</v>
+        <v>277</v>
       </c>
       <c r="J47" s="6" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="K47" s="3" t="s">
         <v>55</v>
@@ -3882,7 +3882,7 @@
         <v>258</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C48" s="7" t="s">
         <v>14</v>
@@ -3897,13 +3897,13 @@
         <v>81</v>
       </c>
       <c r="G48" s="2" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="H48" s="2" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="I48" s="7" t="s">
-        <v>262</v>
+        <v>277</v>
       </c>
       <c r="J48" s="8" t="s">
         <v>259</v>
@@ -3926,7 +3926,7 @@
         <v>192</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C49" s="1" t="s">
         <v>15</v>
@@ -3947,10 +3947,10 @@
         <v>132</v>
       </c>
       <c r="I49" s="1" t="s">
-        <v>262</v>
+        <v>277</v>
       </c>
       <c r="J49" s="1" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="K49" s="3" t="s">
         <v>63</v>
@@ -3970,7 +3970,7 @@
         <v>193</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C50" s="1" t="s">
         <v>15</v>
@@ -3991,10 +3991,10 @@
         <v>132</v>
       </c>
       <c r="I50" s="1" t="s">
-        <v>262</v>
+        <v>277</v>
       </c>
       <c r="J50" s="1" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="K50" s="3" t="s">
         <v>63</v>
@@ -4014,7 +4014,7 @@
         <v>194</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C51" s="1" t="s">
         <v>16</v>
@@ -4035,7 +4035,7 @@
         <v>103</v>
       </c>
       <c r="I51" s="1" t="s">
-        <v>262</v>
+        <v>277</v>
       </c>
       <c r="J51" s="1" t="s">
         <v>61</v>
@@ -4058,7 +4058,7 @@
         <v>195</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C52" s="1" t="s">
         <v>16</v>
@@ -4079,7 +4079,7 @@
         <v>103</v>
       </c>
       <c r="I52" s="1" t="s">
-        <v>262</v>
+        <v>277</v>
       </c>
       <c r="J52" s="1" t="s">
         <v>62</v>
@@ -4102,7 +4102,7 @@
         <v>196</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C53" s="1" t="s">
         <v>18</v>
@@ -4123,10 +4123,10 @@
         <v>104</v>
       </c>
       <c r="I53" s="1" t="s">
-        <v>262</v>
+        <v>277</v>
       </c>
       <c r="J53" s="1" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="K53" s="3" t="s">
         <v>63</v>
@@ -4146,7 +4146,7 @@
         <v>197</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C54" s="1" t="s">
         <v>18</v>
@@ -4167,10 +4167,10 @@
         <v>106</v>
       </c>
       <c r="I54" s="1" t="s">
-        <v>262</v>
+        <v>277</v>
       </c>
       <c r="J54" s="1" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="K54" s="3" t="s">
         <v>63</v>
@@ -4190,7 +4190,7 @@
         <v>198</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C55" s="1" t="s">
         <v>18</v>
@@ -4211,10 +4211,10 @@
         <v>106</v>
       </c>
       <c r="I55" s="1" t="s">
-        <v>262</v>
+        <v>277</v>
       </c>
       <c r="J55" s="1" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="K55" s="3" t="s">
         <v>63</v>
@@ -4234,7 +4234,7 @@
         <v>199</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C56" s="1" t="s">
         <v>18</v>
@@ -4255,10 +4255,10 @@
         <v>106</v>
       </c>
       <c r="I56" s="1" t="s">
-        <v>262</v>
+        <v>277</v>
       </c>
       <c r="J56" s="1" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="K56" s="3" t="s">
         <v>63</v>
@@ -4278,7 +4278,7 @@
         <v>260</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C57" s="1" t="s">
         <v>5</v>
@@ -4299,7 +4299,7 @@
         <v>233</v>
       </c>
       <c r="I57" s="1" t="s">
-        <v>262</v>
+        <v>277</v>
       </c>
       <c r="J57" s="1" t="s">
         <v>64</v>
@@ -4322,7 +4322,7 @@
         <v>200</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C58" s="1" t="s">
         <v>21</v>
@@ -4343,7 +4343,7 @@
         <v>104</v>
       </c>
       <c r="I58" s="1" t="s">
-        <v>262</v>
+        <v>277</v>
       </c>
       <c r="J58" s="1" t="s">
         <v>54</v>
@@ -4363,10 +4363,10 @@
     </row>
     <row r="59" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C59" s="1" t="s">
         <v>22</v>
@@ -4387,7 +4387,7 @@
         <v>104</v>
       </c>
       <c r="I59" s="1" t="s">
-        <v>262</v>
+        <v>277</v>
       </c>
       <c r="J59" s="1" t="s">
         <v>64</v>
@@ -4407,10 +4407,10 @@
     </row>
     <row r="60" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C60" s="1" t="s">
         <v>22</v>
@@ -4431,7 +4431,7 @@
         <v>111</v>
       </c>
       <c r="I60" s="1" t="s">
-        <v>262</v>
+        <v>277</v>
       </c>
       <c r="J60" s="3" t="s">
         <v>2</v>
@@ -4454,7 +4454,7 @@
         <v>201</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C61" s="1" t="s">
         <v>23</v>
@@ -4475,7 +4475,7 @@
         <v>104</v>
       </c>
       <c r="I61" s="1" t="s">
-        <v>262</v>
+        <v>277</v>
       </c>
       <c r="J61" s="1" t="s">
         <v>64</v>
@@ -4498,7 +4498,7 @@
         <v>202</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C62" s="1" t="s">
         <v>23</v>
@@ -4519,7 +4519,7 @@
         <v>111</v>
       </c>
       <c r="I62" s="1" t="s">
-        <v>262</v>
+        <v>277</v>
       </c>
       <c r="J62" s="3" t="s">
         <v>2</v>
@@ -4542,7 +4542,7 @@
         <v>203</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C63" s="1" t="s">
         <v>24</v>
@@ -4563,10 +4563,10 @@
         <v>132</v>
       </c>
       <c r="I63" s="1" t="s">
-        <v>262</v>
+        <v>277</v>
       </c>
       <c r="J63" s="1" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="K63" s="3" t="s">
         <v>55</v>
@@ -4586,7 +4586,7 @@
         <v>204</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C64" s="1" t="s">
         <v>24</v>
@@ -4607,10 +4607,10 @@
         <v>132</v>
       </c>
       <c r="I64" s="1" t="s">
-        <v>262</v>
+        <v>277</v>
       </c>
       <c r="J64" s="1" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="K64" s="3" t="s">
         <v>55</v>
@@ -4630,7 +4630,7 @@
         <v>205</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C65" s="1" t="s">
         <v>25</v>
@@ -4651,7 +4651,7 @@
         <v>132</v>
       </c>
       <c r="I65" s="1" t="s">
-        <v>262</v>
+        <v>277</v>
       </c>
       <c r="J65" s="1" t="s">
         <v>126</v>
@@ -4674,7 +4674,7 @@
         <v>206</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C66" s="1" t="s">
         <v>25</v>
@@ -4695,7 +4695,7 @@
         <v>132</v>
       </c>
       <c r="I66" s="1" t="s">
-        <v>262</v>
+        <v>277</v>
       </c>
       <c r="J66" s="1" t="s">
         <v>126</v>
@@ -4718,7 +4718,7 @@
         <v>207</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C67" s="1" t="s">
         <v>25</v>
@@ -4739,7 +4739,7 @@
         <v>132</v>
       </c>
       <c r="I67" s="1" t="s">
-        <v>262</v>
+        <v>277</v>
       </c>
       <c r="J67" s="1" t="s">
         <v>126</v>
@@ -4762,7 +4762,7 @@
         <v>208</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C68" s="1" t="s">
         <v>25</v>
@@ -4783,7 +4783,7 @@
         <v>132</v>
       </c>
       <c r="I68" s="1" t="s">
-        <v>262</v>
+        <v>277</v>
       </c>
       <c r="J68" s="1" t="s">
         <v>126</v>
@@ -4806,7 +4806,7 @@
         <v>209</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C69" s="1" t="s">
         <v>26</v>
@@ -4827,10 +4827,10 @@
         <v>104</v>
       </c>
       <c r="I69" s="1" t="s">
-        <v>262</v>
+        <v>277</v>
       </c>
       <c r="J69" s="1" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="K69" s="3" t="s">
         <v>55</v>
@@ -4850,7 +4850,7 @@
         <v>210</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C70" s="1" t="s">
         <v>26</v>
@@ -4871,10 +4871,10 @@
         <v>106</v>
       </c>
       <c r="I70" s="1" t="s">
-        <v>262</v>
+        <v>277</v>
       </c>
       <c r="J70" s="1" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="K70" s="3" t="s">
         <v>55</v>
@@ -4894,7 +4894,7 @@
         <v>211</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C71" s="1" t="s">
         <v>26</v>
@@ -4915,10 +4915,10 @@
         <v>106</v>
       </c>
       <c r="I71" s="1" t="s">
-        <v>262</v>
+        <v>277</v>
       </c>
       <c r="J71" s="1" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="K71" s="3" t="s">
         <v>55</v>
@@ -4938,7 +4938,7 @@
         <v>212</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C72" s="1" t="s">
         <v>26</v>
@@ -4959,10 +4959,10 @@
         <v>106</v>
       </c>
       <c r="I72" s="1" t="s">
-        <v>262</v>
+        <v>277</v>
       </c>
       <c r="J72" s="1" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="K72" s="3" t="s">
         <v>55</v>
@@ -4982,7 +4982,7 @@
         <v>213</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C73" s="1" t="s">
         <v>5</v>
@@ -5003,7 +5003,7 @@
         <v>235</v>
       </c>
       <c r="I73" s="1" t="s">
-        <v>262</v>
+        <v>277</v>
       </c>
       <c r="J73" s="1" t="s">
         <v>64</v>
@@ -5026,7 +5026,7 @@
         <v>214</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C74" s="1" t="s">
         <v>27</v>
@@ -5047,10 +5047,10 @@
         <v>105</v>
       </c>
       <c r="I74" s="1" t="s">
-        <v>262</v>
+        <v>277</v>
       </c>
       <c r="J74" s="1" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="K74" s="3" t="s">
         <v>55</v>
@@ -5070,7 +5070,7 @@
         <v>215</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C75" s="1" t="s">
         <v>28</v>
@@ -5091,10 +5091,10 @@
         <v>105</v>
       </c>
       <c r="I75" s="1" t="s">
-        <v>262</v>
+        <v>277</v>
       </c>
       <c r="J75" s="1" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="K75" s="3" t="s">
         <v>55</v>
@@ -5114,7 +5114,7 @@
         <v>216</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C76" s="1" t="s">
         <v>28</v>
@@ -5135,7 +5135,7 @@
         <v>112</v>
       </c>
       <c r="I76" s="1" t="s">
-        <v>262</v>
+        <v>277</v>
       </c>
       <c r="J76" s="3" t="s">
         <v>2</v>
@@ -5158,7 +5158,7 @@
         <v>217</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C77" s="1" t="s">
         <v>27</v>
@@ -5179,7 +5179,7 @@
         <v>112</v>
       </c>
       <c r="I77" s="1" t="s">
-        <v>262</v>
+        <v>277</v>
       </c>
       <c r="J77" s="3" t="s">
         <v>2</v>
@@ -5202,7 +5202,7 @@
         <v>218</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C78" s="2" t="s">
         <v>30</v>
@@ -5223,7 +5223,7 @@
         <v>112</v>
       </c>
       <c r="I78" s="1" t="s">
-        <v>262</v>
+        <v>277</v>
       </c>
       <c r="J78" s="3" t="s">
         <v>2</v>
@@ -5246,7 +5246,7 @@
         <v>219</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C79" s="2" t="s">
         <v>30</v>
@@ -5267,7 +5267,7 @@
         <v>112</v>
       </c>
       <c r="I79" s="1" t="s">
-        <v>262</v>
+        <v>277</v>
       </c>
       <c r="J79" s="3" t="s">
         <v>2</v>
@@ -5290,7 +5290,7 @@
         <v>220</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C80" s="2" t="s">
         <v>30</v>
@@ -5311,10 +5311,10 @@
         <v>134</v>
       </c>
       <c r="I80" s="1" t="s">
-        <v>262</v>
+        <v>277</v>
       </c>
       <c r="J80" s="1" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="K80" s="3" t="s">
         <v>55</v>
@@ -5334,7 +5334,7 @@
         <v>221</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C81" s="2" t="s">
         <v>30</v>
@@ -5355,10 +5355,10 @@
         <v>134</v>
       </c>
       <c r="I81" s="1" t="s">
-        <v>262</v>
+        <v>277</v>
       </c>
       <c r="J81" s="1" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="K81" s="3" t="s">
         <v>55</v>
@@ -5378,7 +5378,7 @@
         <v>222</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C82" s="1" t="s">
         <v>32</v>
@@ -5399,7 +5399,7 @@
         <v>138</v>
       </c>
       <c r="I82" s="1" t="s">
-        <v>262</v>
+        <v>277</v>
       </c>
       <c r="J82" s="1" t="s">
         <v>126</v>
@@ -5422,7 +5422,7 @@
         <v>223</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C83" s="1" t="s">
         <v>32</v>
@@ -5443,7 +5443,7 @@
         <v>138</v>
       </c>
       <c r="I83" s="1" t="s">
-        <v>262</v>
+        <v>277</v>
       </c>
       <c r="J83" s="1" t="s">
         <v>126</v>
@@ -5466,7 +5466,7 @@
         <v>224</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C84" s="1" t="s">
         <v>32</v>
@@ -5487,7 +5487,7 @@
         <v>138</v>
       </c>
       <c r="I84" s="1" t="s">
-        <v>262</v>
+        <v>277</v>
       </c>
       <c r="J84" s="1" t="s">
         <v>126</v>
@@ -5510,7 +5510,7 @@
         <v>225</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C85" s="1" t="s">
         <v>32</v>
@@ -5531,7 +5531,7 @@
         <v>138</v>
       </c>
       <c r="I85" s="1" t="s">
-        <v>262</v>
+        <v>277</v>
       </c>
       <c r="J85" s="1" t="s">
         <v>126</v>
@@ -5554,7 +5554,7 @@
         <v>226</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C86" s="1" t="s">
         <v>34</v>
@@ -5575,10 +5575,10 @@
         <v>105</v>
       </c>
       <c r="I86" s="1" t="s">
-        <v>262</v>
+        <v>277</v>
       </c>
       <c r="J86" s="1" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="K86" s="3" t="s">
         <v>75</v>
@@ -5598,7 +5598,7 @@
         <v>227</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C87" s="1" t="s">
         <v>34</v>
@@ -5619,10 +5619,10 @@
         <v>105</v>
       </c>
       <c r="I87" s="1" t="s">
-        <v>262</v>
+        <v>277</v>
       </c>
       <c r="J87" s="1" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="K87" s="3" t="s">
         <v>75</v>
@@ -5642,7 +5642,7 @@
         <v>228</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C88" s="1" t="s">
         <v>5</v>
@@ -5663,7 +5663,7 @@
         <v>237</v>
       </c>
       <c r="I88" s="1" t="s">
-        <v>262</v>
+        <v>277</v>
       </c>
       <c r="J88" s="1" t="s">
         <v>64</v>
@@ -5686,7 +5686,7 @@
         <v>229</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C89" s="1" t="s">
         <v>34</v>
@@ -5707,10 +5707,10 @@
         <v>105</v>
       </c>
       <c r="I89" s="1" t="s">
-        <v>262</v>
+        <v>277</v>
       </c>
       <c r="J89" s="1" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="K89" s="3" t="s">
         <v>75</v>
@@ -5730,7 +5730,7 @@
         <v>230</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C90" s="9" t="s">
         <v>0</v>
@@ -5751,7 +5751,7 @@
         <v>105</v>
       </c>
       <c r="I90" s="1" t="s">
-        <v>262</v>
+        <v>277</v>
       </c>
       <c r="J90" s="9" t="s">
         <v>64</v>
@@ -5771,10 +5771,10 @@
     </row>
     <row r="91" spans="1:14" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A91" s="11" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C91" s="13" t="s">
         <v>14</v>
@@ -5789,16 +5789,16 @@
         <v>81</v>
       </c>
       <c r="G91" s="11" t="s">
+        <v>272</v>
+      </c>
+      <c r="H91" s="11" t="s">
+        <v>271</v>
+      </c>
+      <c r="I91" s="12" t="s">
+        <v>277</v>
+      </c>
+      <c r="J91" s="6" t="s">
         <v>273</v>
-      </c>
-      <c r="H91" s="11" t="s">
-        <v>272</v>
-      </c>
-      <c r="I91" s="12" t="s">
-        <v>262</v>
-      </c>
-      <c r="J91" s="6" t="s">
-        <v>274</v>
       </c>
       <c r="K91" s="13" t="s">
         <v>63</v>

</xml_diff>

<commit_message>
- add 2024 mer targets
- added 2024 mer targets as per dp-927
</commit_message>
<xml_diff>
--- a/data-raw/snu_x_im_distribution_configuration/23Tto24TMap.xlsx
+++ b/data-raw/snu_x_im_distribution_configuration/23Tto24TMap.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2" conformance="strict">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10808"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10215"/>
   <workbookPr dateCompatibility="0" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jordanbales/Documents/Repos/data-pack-commons/data-raw/snu_x_im_distribution_configuration/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/faustolopezbao/Documents/GitHub/data-pack-commons/data-raw/snu_x_im_distribution_configuration/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{342D3109-669D-8F4D-9468-2894D95148F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{CD1E064A-6AB4-DC4F-BCDB-E1F093A9502E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16000" yWindow="500" windowWidth="32000" windowHeight="26160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="36280" yWindow="1280" windowWidth="35760" windowHeight="17940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Map" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="1274" uniqueCount="270">
+<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="1414" uniqueCount="280">
   <si>
     <t>CXCA_SCRN</t>
   </si>
@@ -846,6 +846,36 @@
   </si>
   <si>
     <t>fy24_age_bands</t>
+  </si>
+  <si>
+    <t>PrEP_CT.TestResult.T</t>
+  </si>
+  <si>
+    <t>DE_GROUP-TXAVaM4oYMd</t>
+  </si>
+  <si>
+    <t>2023Oct</t>
+  </si>
+  <si>
+    <t>HTS.Index.Pos.T</t>
+  </si>
+  <si>
+    <t>HTS.Index.Neg.T</t>
+  </si>
+  <si>
+    <t>HTS_TST.SNS.Pos.T</t>
+  </si>
+  <si>
+    <t>HTS_TST.SNS.Neg.T</t>
+  </si>
+  <si>
+    <t>HTS_TST.ActiveOther.Pos.T</t>
+  </si>
+  <si>
+    <t>HTS_TST.ActiveOther.Neg.T</t>
+  </si>
+  <si>
+    <t>HTS_RECENT.T</t>
   </si>
 </sst>
 </file>
@@ -1005,7 +1035,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1183,6 +1213,12 @@
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -1372,19 +1408,22 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="10" xfId="6" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="10" xfId="7" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="11" xfId="6" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="8" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="10" xfId="8" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="11" xfId="8" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="19" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="33" borderId="10" xfId="6" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1749,18 +1788,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N91"/>
+  <dimension ref="A1:N101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection activeCell="A44" sqref="A44"/>
-      <selection pane="topRight" activeCell="J1" sqref="J1:J1048576"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A74" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D87" sqref="D87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="30.83203125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="23" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.1640625" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.1640625" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.83203125" style="2" customWidth="1"/>
     <col min="5" max="5" width="11.83203125" style="2" bestFit="1" customWidth="1"/>
@@ -1997,7 +2035,7 @@
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="2" t="s">
         <v>147</v>
       </c>
       <c r="B6" s="1" t="s">
@@ -2033,7 +2071,7 @@
       <c r="L6" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="M6" s="4" t="s">
+      <c r="M6" s="2" t="s">
         <v>2</v>
       </c>
       <c r="N6" s="1" t="s">
@@ -2129,7 +2167,7 @@
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A9" s="4" t="s">
+      <c r="A9" s="2" t="s">
         <v>150</v>
       </c>
       <c r="B9" s="1" t="s">
@@ -2165,7 +2203,7 @@
       <c r="L9" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="M9" s="4" t="s">
+      <c r="M9" s="2" t="s">
         <v>2</v>
       </c>
       <c r="N9" s="1" t="s">
@@ -2341,7 +2379,7 @@
       <c r="L13" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="M13" s="4" t="s">
+      <c r="M13" s="2" t="s">
         <v>2</v>
       </c>
       <c r="N13" s="1" t="s">
@@ -2437,7 +2475,7 @@
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A16" s="4" t="s">
+      <c r="A16" s="2" t="s">
         <v>157</v>
       </c>
       <c r="B16" s="1" t="s">
@@ -2473,7 +2511,7 @@
       <c r="L16" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="M16" s="4" t="s">
+      <c r="M16" s="2" t="s">
         <v>2</v>
       </c>
       <c r="N16" s="1" t="s">
@@ -2657,7 +2695,7 @@
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A21" s="4" t="s">
+      <c r="A21" s="2" t="s">
         <v>162</v>
       </c>
       <c r="B21" s="1" t="s">
@@ -2693,7 +2731,7 @@
       <c r="L21" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="M21" s="4" t="s">
+      <c r="M21" s="2" t="s">
         <v>2</v>
       </c>
       <c r="N21" s="1" t="s">
@@ -2825,7 +2863,7 @@
       <c r="L24" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="M24" s="4" t="s">
+      <c r="M24" s="2" t="s">
         <v>2</v>
       </c>
       <c r="N24" s="1" t="s">
@@ -2921,7 +2959,7 @@
       </c>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A27" s="4" t="s">
+      <c r="A27" s="2" t="s">
         <v>168</v>
       </c>
       <c r="B27" s="1" t="s">
@@ -2957,7 +2995,7 @@
       <c r="L27" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="M27" s="4" t="s">
+      <c r="M27" s="2" t="s">
         <v>2</v>
       </c>
       <c r="N27" s="1" t="s">
@@ -3141,7 +3179,7 @@
       </c>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A32" s="4" t="s">
+      <c r="A32" s="2" t="s">
         <v>173</v>
       </c>
       <c r="B32" s="1" t="s">
@@ -3177,7 +3215,7 @@
       <c r="L32" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="M32" s="4" t="s">
+      <c r="M32" s="2" t="s">
         <v>2</v>
       </c>
       <c r="N32" s="1" t="s">
@@ -3273,7 +3311,7 @@
       </c>
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A35" s="4" t="s">
+      <c r="A35" s="2" t="s">
         <v>176</v>
       </c>
       <c r="B35" s="1" t="s">
@@ -3309,7 +3347,7 @@
       <c r="L35" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="M35" s="4" t="s">
+      <c r="M35" s="2" t="s">
         <v>2</v>
       </c>
       <c r="N35" s="1" t="s">
@@ -3441,7 +3479,7 @@
       <c r="L38" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="M38" s="4" t="s">
+      <c r="M38" s="2" t="s">
         <v>2</v>
       </c>
       <c r="N38" s="1" t="s">
@@ -3537,7 +3575,7 @@
       </c>
     </row>
     <row r="41" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A41" s="4" t="s">
+      <c r="A41" s="2" t="s">
         <v>182</v>
       </c>
       <c r="B41" s="1" t="s">
@@ -3617,7 +3655,7 @@
       <c r="L42" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="M42" s="4" t="s">
+      <c r="M42" s="2" t="s">
         <v>2</v>
       </c>
       <c r="N42" s="1" t="s">
@@ -3775,10 +3813,10 @@
       <c r="F46" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="G46" s="5" t="s">
+      <c r="G46" s="4" t="s">
         <v>266</v>
       </c>
-      <c r="H46" s="5" t="s">
+      <c r="H46" s="4" t="s">
         <v>265</v>
       </c>
       <c r="I46" s="1" t="s">
@@ -3819,10 +3857,10 @@
       <c r="F47" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="G47" s="5" t="s">
+      <c r="G47" s="4" t="s">
         <v>266</v>
       </c>
-      <c r="H47" s="5" t="s">
+      <c r="H47" s="4" t="s">
         <v>265</v>
       </c>
       <c r="I47" s="1" t="s">
@@ -3845,22 +3883,22 @@
       </c>
     </row>
     <row r="48" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A48" s="6" t="s">
+      <c r="A48" s="5" t="s">
         <v>254</v>
       </c>
       <c r="B48" s="1" t="s">
         <v>267</v>
       </c>
-      <c r="C48" s="6" t="s">
+      <c r="C48" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D48" s="6" t="s">
+      <c r="D48" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="E48" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="F48" s="6" t="s">
+      <c r="E48" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="F48" s="5" t="s">
         <v>77</v>
       </c>
       <c r="G48" s="2" t="s">
@@ -3869,22 +3907,22 @@
       <c r="H48" s="2" t="s">
         <v>260</v>
       </c>
-      <c r="I48" s="6" t="s">
+      <c r="I48" s="5" t="s">
         <v>268</v>
       </c>
       <c r="J48" t="s">
         <v>269</v>
       </c>
-      <c r="K48" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="L48" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="M48" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="N48" s="6" t="s">
+      <c r="K48" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="L48" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="M48" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="N48" s="5" t="s">
         <v>56</v>
       </c>
     </row>
@@ -4277,7 +4315,7 @@
       <c r="L57" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="M57" s="4" t="s">
+      <c r="M57" s="2" t="s">
         <v>2</v>
       </c>
       <c r="N57" s="1" t="s">
@@ -4945,7 +4983,7 @@
       </c>
     </row>
     <row r="73" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A73" s="4" t="s">
+      <c r="A73" s="2" t="s">
         <v>209</v>
       </c>
       <c r="B73" s="1" t="s">
@@ -4981,7 +5019,7 @@
       <c r="L73" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="M73" s="4" t="s">
+      <c r="M73" s="2" t="s">
         <v>2</v>
       </c>
       <c r="N73" s="1" t="s">
@@ -5605,7 +5643,7 @@
       </c>
     </row>
     <row r="88" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A88" s="4" t="s">
+      <c r="A88" s="2" t="s">
         <v>224</v>
       </c>
       <c r="B88" s="1" t="s">
@@ -5641,7 +5679,7 @@
       <c r="L88" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="M88" s="4" t="s">
+      <c r="M88" s="2" t="s">
         <v>2</v>
       </c>
       <c r="N88" s="1" t="s">
@@ -5699,7 +5737,7 @@
       <c r="B90" s="1" t="s">
         <v>267</v>
       </c>
-      <c r="C90" s="7" t="s">
+      <c r="C90" s="6" t="s">
         <v>0</v>
       </c>
       <c r="D90" s="1" t="s">
@@ -5723,60 +5761,500 @@
       <c r="J90" t="s">
         <v>269</v>
       </c>
-      <c r="K90" s="8" t="s">
+      <c r="K90" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="L90" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="M90" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="N90" s="7" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="91" spans="1:14" s="9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A91" s="9" t="s">
+      <c r="L90" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="M90" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="N90" s="6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="91" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A91" s="8" t="s">
         <v>259</v>
       </c>
       <c r="B91" s="1" t="s">
         <v>267</v>
       </c>
-      <c r="C91" s="11" t="s">
+      <c r="C91" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="D91" s="10" t="s">
+      <c r="D91" s="9" t="s">
         <v>84</v>
       </c>
-      <c r="E91" s="10" t="s">
+      <c r="E91" s="9" t="s">
         <v>36</v>
       </c>
       <c r="F91" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="G91" s="9" t="s">
+      <c r="G91" s="8" t="s">
         <v>263</v>
       </c>
-      <c r="H91" s="9" t="s">
+      <c r="H91" s="8" t="s">
         <v>262</v>
       </c>
-      <c r="I91" s="10" t="s">
+      <c r="I91" s="9" t="s">
         <v>268</v>
       </c>
       <c r="J91" t="s">
         <v>264</v>
       </c>
-      <c r="K91" s="11" t="s">
+      <c r="K91" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="L91" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="M91" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="N91" s="11" t="s">
+      <c r="L91" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="M91" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="N91" s="10" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="92" spans="1:14" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A92" s="11" t="s">
+        <v>270</v>
+      </c>
+      <c r="B92" s="12" t="s">
+        <v>271</v>
+      </c>
+      <c r="C92" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="D92" s="12" t="s">
+        <v>129</v>
+      </c>
+      <c r="E92" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="F92" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="G92" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="H92" s="12" t="s">
+        <v>100</v>
+      </c>
+      <c r="I92" s="12" t="s">
+        <v>272</v>
+      </c>
+      <c r="J92" s="14" t="s">
+        <v>269</v>
+      </c>
+      <c r="K92" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="L92" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="M92" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="N92" s="12" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="93" spans="1:14" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A93" s="11" t="s">
+        <v>273</v>
+      </c>
+      <c r="B93" s="12" t="s">
+        <v>271</v>
+      </c>
+      <c r="C93" s="12" t="s">
+        <v>123</v>
+      </c>
+      <c r="D93" s="12" t="s">
+        <v>124</v>
+      </c>
+      <c r="E93" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="F93" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="G93" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="H93" s="12" t="s">
+        <v>104</v>
+      </c>
+      <c r="I93" s="12" t="s">
+        <v>272</v>
+      </c>
+      <c r="J93" s="14" t="s">
+        <v>269</v>
+      </c>
+      <c r="K93" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="L93" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="M93" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="N93" s="12" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="94" spans="1:14" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A94" s="11" t="s">
+        <v>274</v>
+      </c>
+      <c r="B94" s="12" t="s">
+        <v>271</v>
+      </c>
+      <c r="C94" s="12" t="s">
+        <v>123</v>
+      </c>
+      <c r="D94" s="12" t="s">
+        <v>124</v>
+      </c>
+      <c r="E94" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="F94" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="G94" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="H94" s="12" t="s">
+        <v>104</v>
+      </c>
+      <c r="I94" s="12" t="s">
+        <v>272</v>
+      </c>
+      <c r="J94" s="14" t="s">
+        <v>269</v>
+      </c>
+      <c r="K94" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="L94" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="M94" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="N94" s="12" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="95" spans="1:14" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A95" s="11" t="s">
+        <v>275</v>
+      </c>
+      <c r="B95" s="12" t="s">
+        <v>271</v>
+      </c>
+      <c r="C95" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="D95" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="E95" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="F95" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="G95" s="11" t="s">
+        <v>232</v>
+      </c>
+      <c r="H95" s="11" t="s">
+        <v>233</v>
+      </c>
+      <c r="I95" s="12" t="s">
+        <v>272</v>
+      </c>
+      <c r="J95" s="14" t="s">
+        <v>269</v>
+      </c>
+      <c r="K95" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="L95" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="M95" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="N95" s="12" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="96" spans="1:14" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A96" s="11" t="s">
+        <v>276</v>
+      </c>
+      <c r="B96" s="12" t="s">
+        <v>271</v>
+      </c>
+      <c r="C96" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="D96" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="E96" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="F96" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="G96" s="11" t="s">
+        <v>232</v>
+      </c>
+      <c r="H96" s="11" t="s">
+        <v>233</v>
+      </c>
+      <c r="I96" s="12" t="s">
+        <v>272</v>
+      </c>
+      <c r="J96" s="14" t="s">
+        <v>269</v>
+      </c>
+      <c r="K96" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="L96" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="M96" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="N96" s="12" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="97" spans="1:14" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A97" s="11" t="s">
+        <v>277</v>
+      </c>
+      <c r="B97" s="12" t="s">
+        <v>271</v>
+      </c>
+      <c r="C97" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="D97" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="E97" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="F97" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="G97" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="H97" s="12" t="s">
+        <v>113</v>
+      </c>
+      <c r="I97" s="12" t="s">
+        <v>272</v>
+      </c>
+      <c r="J97" s="14" t="s">
+        <v>269</v>
+      </c>
+      <c r="K97" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="L97" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="M97" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="N97" s="12" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="98" spans="1:14" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A98" s="11" t="s">
+        <v>278</v>
+      </c>
+      <c r="B98" s="12" t="s">
+        <v>271</v>
+      </c>
+      <c r="C98" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="D98" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="E98" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="F98" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="G98" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="H98" s="12" t="s">
+        <v>113</v>
+      </c>
+      <c r="I98" s="12" t="s">
+        <v>272</v>
+      </c>
+      <c r="J98" s="14" t="s">
+        <v>269</v>
+      </c>
+      <c r="K98" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="L98" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="M98" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="N98" s="12" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="99" spans="1:14" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A99" s="11" t="s">
+        <v>279</v>
+      </c>
+      <c r="B99" s="12" t="s">
+        <v>271</v>
+      </c>
+      <c r="C99" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="D99" s="11" t="s">
+        <v>227</v>
+      </c>
+      <c r="E99" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="F99" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="G99" s="11" t="s">
+        <v>232</v>
+      </c>
+      <c r="H99" s="11" t="s">
+        <v>233</v>
+      </c>
+      <c r="I99" s="12" t="s">
+        <v>272</v>
+      </c>
+      <c r="J99" s="14" t="s">
+        <v>269</v>
+      </c>
+      <c r="K99" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="L99" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="M99" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="N99" s="12" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="100" spans="1:14" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A100" s="11" t="s">
+        <v>167</v>
+      </c>
+      <c r="B100" s="12" t="s">
+        <v>271</v>
+      </c>
+      <c r="C100" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="D100" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="E100" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="F100" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="G100" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="H100" s="12" t="s">
+        <v>113</v>
+      </c>
+      <c r="I100" s="12" t="s">
+        <v>272</v>
+      </c>
+      <c r="J100" s="14" t="s">
+        <v>269</v>
+      </c>
+      <c r="K100" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="L100" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="M100" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="N100" s="12" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="101" spans="1:14" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A101" s="11" t="s">
+        <v>166</v>
+      </c>
+      <c r="B101" s="12" t="s">
+        <v>271</v>
+      </c>
+      <c r="C101" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="D101" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="E101" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="F101" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="G101" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="H101" s="12" t="s">
+        <v>113</v>
+      </c>
+      <c r="I101" s="12" t="s">
+        <v>272</v>
+      </c>
+      <c r="J101" s="14" t="s">
+        <v>269</v>
+      </c>
+      <c r="K101" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="L101" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="M101" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="N101" s="12" t="s">
         <v>56</v>
       </c>
     </row>

</xml_diff>

<commit_message>
backed out a single change from dp-858. Line 102 in excelsheet was getting numerator / denominator error.
</commit_message>
<xml_diff>
--- a/data-raw/snu_x_im_distribution_configuration/23Tto24TMap.xlsx
+++ b/data-raw/snu_x_im_distribution_configuration/23Tto24TMap.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jordanbales/Documents/Repos/data-pack-commons/data-raw/snu_x_im_distribution_configuration/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{38B0F1C0-F66E-7145-8B73-932477D46285}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{FBF37D22-2427-734A-B385-A57CDF23925F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="32000" windowHeight="26160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="1428" uniqueCount="283">
+<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="1414" uniqueCount="280">
   <si>
     <t>CXCA_SCRN</t>
   </si>
@@ -875,23 +875,14 @@
     <t>PrEP_CT</t>
   </si>
   <si>
-    <t>PrEP_CT.Neg.T</t>
-  </si>
-  <si>
-    <t>Som9NRMQqV8</t>
-  </si>
-  <si>
     <t>fRWHMVd6Vq5</t>
-  </si>
-  <si>
-    <t>Age/Sex/Result</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="21" x14ac:knownFonts="1">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1042,6 +1033,11 @@
       <sz val="11"/>
       <name val="Lucida Grande"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="13"/>
+      <color rgb="FF202124"/>
+      <name val="Roboto"/>
     </font>
   </fonts>
   <fills count="36">
@@ -1429,7 +1425,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1453,6 +1449,7 @@
     <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="19" fillId="35" borderId="10" xfId="6" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="19" fillId="35" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1817,11 +1814,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N102"/>
+  <dimension ref="A1:N101"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A45" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C92" sqref="C92"/>
+      <pane ySplit="1" topLeftCell="A52" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C60" sqref="C60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4406,7 +4403,7 @@
         <v>278</v>
       </c>
       <c r="D59" s="14" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="E59" s="19" t="s">
         <v>35</v>
@@ -4450,7 +4447,7 @@
         <v>278</v>
       </c>
       <c r="D60" s="14" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="E60" s="19" t="s">
         <v>35</v>
@@ -5858,7 +5855,7 @@
         <v>278</v>
       </c>
       <c r="D92" s="14" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="E92" s="11" t="s">
         <v>35</v>
@@ -6199,7 +6196,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="100" spans="1:14" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:14" s="11" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A100" s="11" t="s">
         <v>165</v>
       </c>
@@ -6218,8 +6215,8 @@
       <c r="F100" s="12" t="s">
         <v>76</v>
       </c>
-      <c r="G100" s="12" t="s">
-        <v>282</v>
+      <c r="G100" s="23" t="s">
+        <v>37</v>
       </c>
       <c r="H100" s="12" t="s">
         <v>112</v>
@@ -6243,7 +6240,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="101" spans="1:14" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:14" s="11" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A101" s="11" t="s">
         <v>164</v>
       </c>
@@ -6262,8 +6259,8 @@
       <c r="F101" s="12" t="s">
         <v>76</v>
       </c>
-      <c r="G101" s="12" t="s">
-        <v>282</v>
+      <c r="G101" s="23" t="s">
+        <v>37</v>
       </c>
       <c r="H101" s="12" t="s">
         <v>112</v>
@@ -6284,50 +6281,6 @@
         <v>2</v>
       </c>
       <c r="N101" s="12" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="102" spans="1:14" s="11" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A102" s="11" t="s">
-        <v>279</v>
-      </c>
-      <c r="B102" s="12" t="s">
-        <v>269</v>
-      </c>
-      <c r="C102" s="11" t="s">
-        <v>278</v>
-      </c>
-      <c r="D102" s="14" t="s">
-        <v>281</v>
-      </c>
-      <c r="E102" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="F102" s="12" t="s">
-        <v>280</v>
-      </c>
-      <c r="G102" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="H102" s="12" t="s">
-        <v>100</v>
-      </c>
-      <c r="I102" s="11" t="s">
-        <v>270</v>
-      </c>
-      <c r="J102" s="14" t="s">
-        <v>267</v>
-      </c>
-      <c r="K102" s="13" t="s">
-        <v>53</v>
-      </c>
-      <c r="L102" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="M102" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="N102" s="12" t="s">
         <v>55</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Files created against Datim. Updated ALL rows in the period column to be 2022Oct Updated prepcttestresult to be Age/Sex NOT Age/Sex/HIVStatus
</commit_message>
<xml_diff>
--- a/data-raw/snu_x_im_distribution_configuration/23Tto24TMap.xlsx
+++ b/data-raw/snu_x_im_distribution_configuration/23Tto24TMap.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2" conformance="strict">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10215"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10808"/>
   <workbookPr dateCompatibility="0" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/faustolopezbao/Documents/GitHub/data-pack-commons/data-raw/snu_x_im_distribution_configuration/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jordanbales/Documents/Repos/data-pack-commons/data-raw/snu_x_im_distribution_configuration/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{638F6A4F-990E-8E48-86F7-D46F73F33412}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{D4707B4A-0660-EB4A-9C64-B5ED86729C4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="37240" yWindow="1260" windowWidth="32000" windowHeight="20340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="16000" yWindow="500" windowWidth="32000" windowHeight="26160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Map" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="1414" uniqueCount="280">
+<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="1414" uniqueCount="279">
   <si>
     <t>CXCA_SCRN</t>
   </si>
@@ -846,9 +846,6 @@
   </si>
   <si>
     <t>DE_GROUP-TXAVaM4oYMd</t>
-  </si>
-  <si>
-    <t>2023Oct</t>
   </si>
   <si>
     <t>HTS.Index.Pos.T</t>
@@ -1817,8 +1814,8 @@
   <dimension ref="A1:N101"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A63" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F96" sqref="F96"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H96" sqref="H96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4400,10 +4397,10 @@
         <v>265</v>
       </c>
       <c r="C59" s="11" t="s">
+        <v>277</v>
+      </c>
+      <c r="D59" s="14" t="s">
         <v>278</v>
-      </c>
-      <c r="D59" s="14" t="s">
-        <v>279</v>
       </c>
       <c r="E59" s="15" t="s">
         <v>35</v>
@@ -4444,10 +4441,10 @@
         <v>265</v>
       </c>
       <c r="C60" s="11" t="s">
+        <v>277</v>
+      </c>
+      <c r="D60" s="14" t="s">
         <v>278</v>
-      </c>
-      <c r="D60" s="14" t="s">
-        <v>279</v>
       </c>
       <c r="E60" s="15" t="s">
         <v>35</v>
@@ -5852,25 +5849,25 @@
         <v>269</v>
       </c>
       <c r="C92" s="11" t="s">
+        <v>277</v>
+      </c>
+      <c r="D92" s="14" t="s">
         <v>278</v>
       </c>
-      <c r="D92" s="14" t="s">
-        <v>279</v>
-      </c>
       <c r="E92" s="11" t="s">
         <v>35</v>
       </c>
       <c r="F92" s="12" t="s">
         <v>76</v>
       </c>
-      <c r="G92" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="H92" s="12" t="s">
-        <v>100</v>
+      <c r="G92" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="H92" s="15" t="s">
+        <v>99</v>
       </c>
       <c r="I92" s="12" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="J92" s="14" t="s">
         <v>267</v>
@@ -5890,7 +5887,7 @@
     </row>
     <row r="93" spans="1:14" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A93" s="11" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B93" s="12" t="s">
         <v>269</v>
@@ -5914,7 +5911,7 @@
         <v>103</v>
       </c>
       <c r="I93" s="12" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="J93" s="14" t="s">
         <v>267</v>
@@ -5934,7 +5931,7 @@
     </row>
     <row r="94" spans="1:14" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A94" s="11" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B94" s="12" t="s">
         <v>269</v>
@@ -5958,7 +5955,7 @@
         <v>103</v>
       </c>
       <c r="I94" s="12" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="J94" s="14" t="s">
         <v>267</v>
@@ -5978,7 +5975,7 @@
     </row>
     <row r="95" spans="1:14" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A95" s="11" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B95" s="12" t="s">
         <v>269</v>
@@ -6002,7 +5999,7 @@
         <v>231</v>
       </c>
       <c r="I95" s="12" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="J95" s="14" t="s">
         <v>267</v>
@@ -6022,7 +6019,7 @@
     </row>
     <row r="96" spans="1:14" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A96" s="11" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B96" s="12" t="s">
         <v>269</v>
@@ -6046,7 +6043,7 @@
         <v>231</v>
       </c>
       <c r="I96" s="12" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="J96" s="14" t="s">
         <v>267</v>
@@ -6066,7 +6063,7 @@
     </row>
     <row r="97" spans="1:14" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A97" s="11" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B97" s="12" t="s">
         <v>269</v>
@@ -6090,7 +6087,7 @@
         <v>112</v>
       </c>
       <c r="I97" s="12" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="J97" s="14" t="s">
         <v>267</v>
@@ -6110,7 +6107,7 @@
     </row>
     <row r="98" spans="1:14" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A98" s="11" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B98" s="12" t="s">
         <v>269</v>
@@ -6134,7 +6131,7 @@
         <v>112</v>
       </c>
       <c r="I98" s="12" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="J98" s="14" t="s">
         <v>267</v>
@@ -6154,7 +6151,7 @@
     </row>
     <row r="99" spans="1:14" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A99" s="11" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B99" s="12" t="s">
         <v>269</v>
@@ -6178,7 +6175,7 @@
         <v>231</v>
       </c>
       <c r="I99" s="12" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="J99" s="14" t="s">
         <v>267</v>
@@ -6222,7 +6219,7 @@
         <v>112</v>
       </c>
       <c r="I100" s="12" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="J100" s="14" t="s">
         <v>267</v>
@@ -6266,7 +6263,7 @@
         <v>112</v>
       </c>
       <c r="I101" s="12" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="J101" s="14" t="s">
         <v>267</v>

</xml_diff>

<commit_message>
DP-927 added modalities for different indicators
-as per DP-927 resolving the addition of modalities for new indicators
</commit_message>
<xml_diff>
--- a/data-raw/snu_x_im_distribution_configuration/23Tto24TMap.xlsx
+++ b/data-raw/snu_x_im_distribution_configuration/23Tto24TMap.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2" conformance="strict">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10215"/>
   <workbookPr dateCompatibility="0" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sam/Documents/GitHub/data-pack-commons/data-raw/snu_x_im_distribution_configuration/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/faustolopezbao/Documents/GitHub/data-pack-commons/data-raw/snu_x_im_distribution_configuration/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{57F6702A-9BE1-0344-A122-A5EFD472E837}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{81DFC993-7113-534A-B18A-3BDA55AB6D79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1600" yWindow="500" windowWidth="32000" windowHeight="20340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="36060" yWindow="1040" windowWidth="37520" windowHeight="18980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Map" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="1414" uniqueCount="280">
+<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="1414" uniqueCount="286">
   <si>
     <t>CXCA_SCRN</t>
   </si>
@@ -876,6 +876,24 @@
   </si>
   <si>
     <t>zzNslrLngKi;xds87opkbem</t>
+  </si>
+  <si>
+    <t>OtherMod/Age Aggregated/Sex/Result;MobileMod/Age/Sex/Result</t>
+  </si>
+  <si>
+    <t>cYRowDkVEpl;Qr9eyrVLHSg</t>
+  </si>
+  <si>
+    <t>IndexMod/Age/Sex/HIVStatus;Index/Age/Sex/HIVStatus;Emergency Ward/Age/Sex/HIVStatus;Inpat/Age/Sex/HIVStatus;MobileMod/Age/Sex/HIVStatus;OtherMod/Age/Sex/HIVStatus;OtherPITC/Age/Sex/HIVStatus;PMTCT PostANC/Age/Sex/HIVStatus;STI Clinic/Age/Sex/HIVStatus;VCT/Age/Sex/HIVStatus;KeyPop/HIVStatus;PMTCT ANC/Age/Sex/HIVStatus;TBClinic/Age/Sex/HIVStatus;VMMC/Age/Sex/HIVStatus</t>
+  </si>
+  <si>
+    <t>cnlEjFkl5UZ;Tpc0Ztxae9H;lJQyt3PjrVy;CEcYYCkTncR;EVwSAwSEfTg;G6QgzwFMWSP;Y3aCLwI6IU3;c60fuhOWPu4;WGV3YTTqrZ3;vYZLPZAuv8A;oLVJbdHt6ou;FazeYvGkStI;PcsTdqSq0Id;mCtbMQYjHjj</t>
+  </si>
+  <si>
+    <t>Inpat/Age/Sex/Result;Emergency Ward/Age/Sex/Result;OtherPITC/Age/Sex/Result;VCT/Age/Sex/Result;Pediatric/Age/Sex/Result;Malnutrition/Age/Sex/Result</t>
+  </si>
+  <si>
+    <t>p6j1mfN4rjP;iPfNX6Ylqp1;E3VaSq4JOzd;dcaYk7TXk4E;iFlQUEQcsfZ;jEpJPF6IVVB</t>
   </si>
 </sst>
 </file>
@@ -1040,7 +1058,7 @@
       <name val="Roboto"/>
     </font>
   </fonts>
-  <fills count="37">
+  <fills count="38">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1240,7 +1258,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF92D050"/>
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1431,7 +1455,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1444,8 +1468,6 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="10" xfId="8" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="11" xfId="8" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="19" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="19" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="19" fillId="33" borderId="10" xfId="6" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="19" fillId="34" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
@@ -1455,11 +1477,23 @@
     <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="19" fillId="35" borderId="10" xfId="6" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="19" fillId="35" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="21" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="19" fillId="36" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="19" fillId="36" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="19" fillId="36" borderId="10" xfId="6" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="36" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="36" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="36" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="37" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="19" fillId="37" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="19" fillId="37" borderId="10" xfId="6" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1826,16 +1860,16 @@
 <worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N101"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A80" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A93" sqref="A93"/>
+    <sheetView tabSelected="1" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A85" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G99" sqref="G99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="30.83203125" style="2" customWidth="1"/>
     <col min="2" max="2" width="24.1640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.6640625" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.83203125" style="2" customWidth="1"/>
     <col min="5" max="5" width="11.83203125" style="2" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15.83203125" style="2" customWidth="1"/>
@@ -1982,267 +2016,267 @@
         <v>55</v>
       </c>
     </row>
-    <row r="4" spans="1:14" s="22" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="19" t="s">
+    <row r="4" spans="1:14" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="17" t="s">
         <v>143</v>
       </c>
-      <c r="B4" s="19" t="s">
-        <v>265</v>
-      </c>
-      <c r="C4" s="19" t="s">
+      <c r="B4" s="17" t="s">
+        <v>265</v>
+      </c>
+      <c r="C4" s="17" t="s">
         <v>122</v>
       </c>
-      <c r="D4" s="19" t="s">
+      <c r="D4" s="17" t="s">
         <v>123</v>
       </c>
-      <c r="E4" s="19" t="s">
-        <v>35</v>
-      </c>
-      <c r="F4" s="19" t="s">
-        <v>76</v>
-      </c>
-      <c r="G4" s="19" t="s">
+      <c r="E4" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="F4" s="17" t="s">
+        <v>76</v>
+      </c>
+      <c r="G4" s="17" t="s">
         <v>44</v>
       </c>
-      <c r="H4" s="19" t="s">
+      <c r="H4" s="17" t="s">
         <v>104</v>
       </c>
-      <c r="I4" s="19" t="s">
-        <v>266</v>
-      </c>
-      <c r="J4" s="20" t="s">
-        <v>267</v>
-      </c>
-      <c r="K4" s="21" t="s">
-        <v>53</v>
-      </c>
-      <c r="L4" s="21" t="s">
-        <v>2</v>
-      </c>
-      <c r="M4" s="22" t="s">
+      <c r="I4" s="17" t="s">
+        <v>266</v>
+      </c>
+      <c r="J4" s="18" t="s">
+        <v>267</v>
+      </c>
+      <c r="K4" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="L4" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="M4" s="20" t="s">
         <v>67</v>
       </c>
-      <c r="N4" s="19" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" s="22" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="19" t="s">
+      <c r="N4" s="17" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="17" t="s">
         <v>144</v>
       </c>
-      <c r="B5" s="19" t="s">
-        <v>265</v>
-      </c>
-      <c r="C5" s="19" t="s">
+      <c r="B5" s="17" t="s">
+        <v>265</v>
+      </c>
+      <c r="C5" s="17" t="s">
         <v>122</v>
       </c>
-      <c r="D5" s="19" t="s">
+      <c r="D5" s="17" t="s">
         <v>123</v>
       </c>
-      <c r="E5" s="19" t="s">
-        <v>35</v>
-      </c>
-      <c r="F5" s="19" t="s">
-        <v>76</v>
-      </c>
-      <c r="G5" s="19" t="s">
+      <c r="E5" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="F5" s="17" t="s">
+        <v>76</v>
+      </c>
+      <c r="G5" s="17" t="s">
         <v>44</v>
       </c>
-      <c r="H5" s="19" t="s">
+      <c r="H5" s="17" t="s">
         <v>104</v>
       </c>
-      <c r="I5" s="19" t="s">
-        <v>266</v>
-      </c>
-      <c r="J5" s="20" t="s">
-        <v>267</v>
-      </c>
-      <c r="K5" s="21" t="s">
-        <v>53</v>
-      </c>
-      <c r="L5" s="21" t="s">
-        <v>2</v>
-      </c>
-      <c r="M5" s="22" t="s">
+      <c r="I5" s="17" t="s">
+        <v>266</v>
+      </c>
+      <c r="J5" s="18" t="s">
+        <v>267</v>
+      </c>
+      <c r="K5" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="L5" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="M5" s="20" t="s">
         <v>68</v>
       </c>
-      <c r="N5" s="19" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" s="22" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="22" t="s">
+      <c r="N5" s="17" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="20" t="s">
         <v>145</v>
       </c>
-      <c r="B6" s="19" t="s">
-        <v>265</v>
-      </c>
-      <c r="C6" s="19" t="s">
+      <c r="B6" s="17" t="s">
+        <v>265</v>
+      </c>
+      <c r="C6" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="22" t="s">
+      <c r="D6" s="20" t="s">
         <v>225</v>
       </c>
-      <c r="E6" s="19" t="s">
-        <v>35</v>
-      </c>
-      <c r="F6" s="19" t="s">
-        <v>76</v>
-      </c>
-      <c r="G6" s="19" t="s">
+      <c r="E6" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="F6" s="17" t="s">
+        <v>76</v>
+      </c>
+      <c r="G6" s="17" t="s">
         <v>232</v>
       </c>
-      <c r="H6" s="22" t="s">
+      <c r="H6" s="20" t="s">
         <v>242</v>
       </c>
-      <c r="I6" s="19" t="s">
-        <v>266</v>
-      </c>
-      <c r="J6" s="20" t="s">
-        <v>267</v>
-      </c>
-      <c r="K6" s="21" t="s">
-        <v>53</v>
-      </c>
-      <c r="L6" s="21" t="s">
-        <v>2</v>
-      </c>
-      <c r="M6" s="22" t="s">
-        <v>2</v>
-      </c>
-      <c r="N6" s="19" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" s="22" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="19" t="s">
+      <c r="I6" s="17" t="s">
+        <v>266</v>
+      </c>
+      <c r="J6" s="18" t="s">
+        <v>267</v>
+      </c>
+      <c r="K6" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="L6" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="M6" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="N6" s="17" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="17" t="s">
         <v>146</v>
       </c>
-      <c r="B7" s="19" t="s">
-        <v>265</v>
-      </c>
-      <c r="C7" s="19" t="s">
+      <c r="B7" s="17" t="s">
+        <v>265</v>
+      </c>
+      <c r="C7" s="17" t="s">
         <v>122</v>
       </c>
-      <c r="D7" s="19" t="s">
+      <c r="D7" s="17" t="s">
         <v>123</v>
       </c>
-      <c r="E7" s="19" t="s">
-        <v>35</v>
-      </c>
-      <c r="F7" s="19" t="s">
-        <v>76</v>
-      </c>
-      <c r="G7" s="19" t="s">
+      <c r="E7" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="F7" s="17" t="s">
+        <v>76</v>
+      </c>
+      <c r="G7" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="H7" s="19" t="s">
+      <c r="H7" s="17" t="s">
         <v>103</v>
       </c>
-      <c r="I7" s="19" t="s">
-        <v>266</v>
-      </c>
-      <c r="J7" s="20" t="s">
-        <v>267</v>
-      </c>
-      <c r="K7" s="21" t="s">
-        <v>53</v>
-      </c>
-      <c r="L7" s="21" t="s">
-        <v>2</v>
-      </c>
-      <c r="M7" s="22" t="s">
+      <c r="I7" s="17" t="s">
+        <v>266</v>
+      </c>
+      <c r="J7" s="18" t="s">
+        <v>267</v>
+      </c>
+      <c r="K7" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="L7" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="M7" s="20" t="s">
         <v>67</v>
       </c>
-      <c r="N7" s="19" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" s="22" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="19" t="s">
+      <c r="N7" s="17" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="17" t="s">
         <v>147</v>
       </c>
-      <c r="B8" s="19" t="s">
-        <v>265</v>
-      </c>
-      <c r="C8" s="19" t="s">
+      <c r="B8" s="17" t="s">
+        <v>265</v>
+      </c>
+      <c r="C8" s="17" t="s">
         <v>122</v>
       </c>
-      <c r="D8" s="19" t="s">
+      <c r="D8" s="17" t="s">
         <v>123</v>
       </c>
-      <c r="E8" s="19" t="s">
-        <v>35</v>
-      </c>
-      <c r="F8" s="19" t="s">
-        <v>76</v>
-      </c>
-      <c r="G8" s="19" t="s">
+      <c r="E8" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="F8" s="17" t="s">
+        <v>76</v>
+      </c>
+      <c r="G8" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="H8" s="19" t="s">
+      <c r="H8" s="17" t="s">
         <v>103</v>
       </c>
-      <c r="I8" s="19" t="s">
-        <v>266</v>
-      </c>
-      <c r="J8" s="20" t="s">
-        <v>267</v>
-      </c>
-      <c r="K8" s="21" t="s">
-        <v>53</v>
-      </c>
-      <c r="L8" s="21" t="s">
-        <v>2</v>
-      </c>
-      <c r="M8" s="22" t="s">
+      <c r="I8" s="17" t="s">
+        <v>266</v>
+      </c>
+      <c r="J8" s="18" t="s">
+        <v>267</v>
+      </c>
+      <c r="K8" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="L8" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="M8" s="20" t="s">
         <v>68</v>
       </c>
-      <c r="N8" s="19" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" s="22" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="22" t="s">
+      <c r="N8" s="17" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="20" t="s">
         <v>148</v>
       </c>
-      <c r="B9" s="19" t="s">
-        <v>265</v>
-      </c>
-      <c r="C9" s="19" t="s">
+      <c r="B9" s="17" t="s">
+        <v>265</v>
+      </c>
+      <c r="C9" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="D9" s="22" t="s">
+      <c r="D9" s="20" t="s">
         <v>225</v>
       </c>
-      <c r="E9" s="19" t="s">
-        <v>35</v>
-      </c>
-      <c r="F9" s="19" t="s">
-        <v>76</v>
-      </c>
-      <c r="G9" s="19" t="s">
+      <c r="E9" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="F9" s="17" t="s">
+        <v>76</v>
+      </c>
+      <c r="G9" s="17" t="s">
         <v>233</v>
       </c>
-      <c r="H9" s="22" t="s">
+      <c r="H9" s="20" t="s">
         <v>243</v>
       </c>
-      <c r="I9" s="19" t="s">
-        <v>266</v>
-      </c>
-      <c r="J9" s="20" t="s">
-        <v>267</v>
-      </c>
-      <c r="K9" s="21" t="s">
-        <v>53</v>
-      </c>
-      <c r="L9" s="21" t="s">
-        <v>2</v>
-      </c>
-      <c r="M9" s="22" t="s">
-        <v>2</v>
-      </c>
-      <c r="N9" s="19" t="s">
+      <c r="I9" s="17" t="s">
+        <v>266</v>
+      </c>
+      <c r="J9" s="18" t="s">
+        <v>267</v>
+      </c>
+      <c r="K9" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="L9" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="M9" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="N9" s="17" t="s">
         <v>55</v>
       </c>
     </row>
@@ -2290,619 +2324,619 @@
         <v>55</v>
       </c>
     </row>
-    <row r="11" spans="1:14" s="22" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="19" t="s">
+    <row r="11" spans="1:14" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="17" t="s">
         <v>150</v>
       </c>
-      <c r="B11" s="19" t="s">
-        <v>265</v>
-      </c>
-      <c r="C11" s="19" t="s">
+      <c r="B11" s="17" t="s">
+        <v>265</v>
+      </c>
+      <c r="C11" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="D11" s="19" t="s">
+      <c r="D11" s="17" t="s">
         <v>79</v>
       </c>
-      <c r="E11" s="19" t="s">
-        <v>35</v>
-      </c>
-      <c r="F11" s="19" t="s">
-        <v>76</v>
-      </c>
-      <c r="G11" s="19" t="s">
+      <c r="E11" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="F11" s="17" t="s">
+        <v>76</v>
+      </c>
+      <c r="G11" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="H11" s="19" t="s">
+      <c r="H11" s="17" t="s">
         <v>102</v>
       </c>
-      <c r="I11" s="19" t="s">
-        <v>266</v>
-      </c>
-      <c r="J11" s="20" t="s">
-        <v>267</v>
-      </c>
-      <c r="K11" s="21" t="s">
-        <v>53</v>
-      </c>
-      <c r="L11" s="21" t="s">
-        <v>2</v>
-      </c>
-      <c r="M11" s="19" t="s">
+      <c r="I11" s="17" t="s">
+        <v>266</v>
+      </c>
+      <c r="J11" s="18" t="s">
+        <v>267</v>
+      </c>
+      <c r="K11" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="L11" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="M11" s="17" t="s">
         <v>62</v>
       </c>
-      <c r="N11" s="19" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" s="22" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="19" t="s">
+      <c r="N11" s="17" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="17" t="s">
         <v>151</v>
       </c>
-      <c r="B12" s="19" t="s">
-        <v>265</v>
-      </c>
-      <c r="C12" s="19" t="s">
+      <c r="B12" s="17" t="s">
+        <v>265</v>
+      </c>
+      <c r="C12" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="D12" s="19" t="s">
+      <c r="D12" s="17" t="s">
         <v>79</v>
       </c>
-      <c r="E12" s="19" t="s">
-        <v>35</v>
-      </c>
-      <c r="F12" s="19" t="s">
-        <v>76</v>
-      </c>
-      <c r="G12" s="19" t="s">
+      <c r="E12" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="F12" s="17" t="s">
+        <v>76</v>
+      </c>
+      <c r="G12" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="H12" s="19" t="s">
+      <c r="H12" s="17" t="s">
         <v>102</v>
       </c>
-      <c r="I12" s="19" t="s">
-        <v>266</v>
-      </c>
-      <c r="J12" s="20" t="s">
-        <v>267</v>
-      </c>
-      <c r="K12" s="21" t="s">
-        <v>53</v>
-      </c>
-      <c r="L12" s="21" t="s">
-        <v>2</v>
-      </c>
-      <c r="M12" s="19" t="s">
+      <c r="I12" s="17" t="s">
+        <v>266</v>
+      </c>
+      <c r="J12" s="18" t="s">
+        <v>267</v>
+      </c>
+      <c r="K12" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="L12" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="M12" s="17" t="s">
         <v>63</v>
       </c>
-      <c r="N12" s="19" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" s="22" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="22" t="s">
+      <c r="N12" s="17" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="20" t="s">
         <v>152</v>
       </c>
-      <c r="B13" s="19" t="s">
-        <v>265</v>
-      </c>
-      <c r="C13" s="19" t="s">
+      <c r="B13" s="17" t="s">
+        <v>265</v>
+      </c>
+      <c r="C13" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="D13" s="22" t="s">
+      <c r="D13" s="20" t="s">
         <v>225</v>
       </c>
-      <c r="E13" s="19" t="s">
-        <v>35</v>
-      </c>
-      <c r="F13" s="19" t="s">
-        <v>76</v>
-      </c>
-      <c r="G13" s="19" t="s">
+      <c r="E13" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="F13" s="17" t="s">
+        <v>76</v>
+      </c>
+      <c r="G13" s="17" t="s">
         <v>234</v>
       </c>
-      <c r="H13" s="22" t="s">
+      <c r="H13" s="20" t="s">
         <v>244</v>
       </c>
-      <c r="I13" s="19" t="s">
-        <v>266</v>
-      </c>
-      <c r="J13" s="20" t="s">
-        <v>267</v>
-      </c>
-      <c r="K13" s="21" t="s">
-        <v>53</v>
-      </c>
-      <c r="L13" s="21" t="s">
-        <v>2</v>
-      </c>
-      <c r="M13" s="22" t="s">
-        <v>2</v>
-      </c>
-      <c r="N13" s="19" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" s="22" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="19" t="s">
+      <c r="I13" s="17" t="s">
+        <v>266</v>
+      </c>
+      <c r="J13" s="18" t="s">
+        <v>267</v>
+      </c>
+      <c r="K13" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="L13" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="M13" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="N13" s="17" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="17" t="s">
         <v>153</v>
       </c>
-      <c r="B14" s="19" t="s">
-        <v>265</v>
-      </c>
-      <c r="C14" s="19" t="s">
+      <c r="B14" s="17" t="s">
+        <v>265</v>
+      </c>
+      <c r="C14" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="D14" s="19" t="s">
+      <c r="D14" s="17" t="s">
         <v>79</v>
       </c>
-      <c r="E14" s="19" t="s">
-        <v>35</v>
-      </c>
-      <c r="F14" s="19" t="s">
-        <v>76</v>
-      </c>
-      <c r="G14" s="19" t="s">
+      <c r="E14" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="F14" s="17" t="s">
+        <v>76</v>
+      </c>
+      <c r="G14" s="17" t="s">
         <v>46</v>
       </c>
-      <c r="H14" s="19" t="s">
+      <c r="H14" s="17" t="s">
         <v>105</v>
       </c>
-      <c r="I14" s="19" t="s">
-        <v>266</v>
-      </c>
-      <c r="J14" s="20" t="s">
-        <v>267</v>
-      </c>
-      <c r="K14" s="21" t="s">
-        <v>53</v>
-      </c>
-      <c r="L14" s="21" t="s">
-        <v>2</v>
-      </c>
-      <c r="M14" s="19" t="s">
+      <c r="I14" s="17" t="s">
+        <v>266</v>
+      </c>
+      <c r="J14" s="18" t="s">
+        <v>267</v>
+      </c>
+      <c r="K14" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="L14" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="M14" s="17" t="s">
         <v>62</v>
       </c>
-      <c r="N14" s="19" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14" s="22" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="19" t="s">
+      <c r="N14" s="17" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="17" t="s">
         <v>154</v>
       </c>
-      <c r="B15" s="19" t="s">
-        <v>265</v>
-      </c>
-      <c r="C15" s="19" t="s">
+      <c r="B15" s="17" t="s">
+        <v>265</v>
+      </c>
+      <c r="C15" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="D15" s="19" t="s">
+      <c r="D15" s="17" t="s">
         <v>79</v>
       </c>
-      <c r="E15" s="19" t="s">
-        <v>35</v>
-      </c>
-      <c r="F15" s="19" t="s">
-        <v>76</v>
-      </c>
-      <c r="G15" s="19" t="s">
+      <c r="E15" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="F15" s="17" t="s">
+        <v>76</v>
+      </c>
+      <c r="G15" s="17" t="s">
         <v>46</v>
       </c>
-      <c r="H15" s="19" t="s">
+      <c r="H15" s="17" t="s">
         <v>105</v>
       </c>
-      <c r="I15" s="19" t="s">
-        <v>266</v>
-      </c>
-      <c r="J15" s="20" t="s">
-        <v>267</v>
-      </c>
-      <c r="K15" s="21" t="s">
-        <v>53</v>
-      </c>
-      <c r="L15" s="21" t="s">
-        <v>2</v>
-      </c>
-      <c r="M15" s="19" t="s">
+      <c r="I15" s="17" t="s">
+        <v>266</v>
+      </c>
+      <c r="J15" s="18" t="s">
+        <v>267</v>
+      </c>
+      <c r="K15" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="L15" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="M15" s="17" t="s">
         <v>63</v>
       </c>
-      <c r="N15" s="19" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14" s="22" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="22" t="s">
+      <c r="N15" s="17" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="20" t="s">
         <v>155</v>
       </c>
-      <c r="B16" s="19" t="s">
-        <v>265</v>
-      </c>
-      <c r="C16" s="19" t="s">
+      <c r="B16" s="17" t="s">
+        <v>265</v>
+      </c>
+      <c r="C16" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="D16" s="22" t="s">
+      <c r="D16" s="20" t="s">
         <v>225</v>
       </c>
-      <c r="E16" s="19" t="s">
-        <v>35</v>
-      </c>
-      <c r="F16" s="19" t="s">
-        <v>76</v>
-      </c>
-      <c r="G16" s="19" t="s">
+      <c r="E16" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="F16" s="17" t="s">
+        <v>76</v>
+      </c>
+      <c r="G16" s="17" t="s">
         <v>235</v>
       </c>
-      <c r="H16" s="22" t="s">
+      <c r="H16" s="20" t="s">
         <v>245</v>
       </c>
-      <c r="I16" s="19" t="s">
-        <v>266</v>
-      </c>
-      <c r="J16" s="20" t="s">
-        <v>267</v>
-      </c>
-      <c r="K16" s="21" t="s">
-        <v>53</v>
-      </c>
-      <c r="L16" s="21" t="s">
-        <v>2</v>
-      </c>
-      <c r="M16" s="22" t="s">
-        <v>2</v>
-      </c>
-      <c r="N16" s="19" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="17" spans="1:14" s="22" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="19" t="s">
+      <c r="I16" s="17" t="s">
+        <v>266</v>
+      </c>
+      <c r="J16" s="18" t="s">
+        <v>267</v>
+      </c>
+      <c r="K16" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="L16" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="M16" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="N16" s="17" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="17" t="s">
         <v>156</v>
       </c>
-      <c r="B17" s="19" t="s">
-        <v>265</v>
-      </c>
-      <c r="C17" s="19" t="s">
+      <c r="B17" s="17" t="s">
+        <v>265</v>
+      </c>
+      <c r="C17" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="D17" s="19" t="s">
+      <c r="D17" s="17" t="s">
         <v>79</v>
       </c>
-      <c r="E17" s="19" t="s">
-        <v>35</v>
-      </c>
-      <c r="F17" s="19" t="s">
-        <v>76</v>
-      </c>
-      <c r="G17" s="19" t="s">
+      <c r="E17" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="F17" s="17" t="s">
+        <v>76</v>
+      </c>
+      <c r="G17" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="H17" s="19" t="s">
+      <c r="H17" s="17" t="s">
         <v>109</v>
       </c>
-      <c r="I17" s="19" t="s">
-        <v>266</v>
-      </c>
-      <c r="J17" s="20" t="s">
-        <v>267</v>
-      </c>
-      <c r="K17" s="21" t="s">
-        <v>53</v>
-      </c>
-      <c r="L17" s="21" t="s">
-        <v>2</v>
-      </c>
-      <c r="M17" s="19" t="s">
+      <c r="I17" s="17" t="s">
+        <v>266</v>
+      </c>
+      <c r="J17" s="18" t="s">
+        <v>267</v>
+      </c>
+      <c r="K17" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="L17" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="M17" s="17" t="s">
         <v>62</v>
       </c>
-      <c r="N17" s="19" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="18" spans="1:14" s="22" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="19" t="s">
+      <c r="N17" s="17" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="17" t="s">
         <v>157</v>
       </c>
-      <c r="B18" s="19" t="s">
-        <v>265</v>
-      </c>
-      <c r="C18" s="19" t="s">
+      <c r="B18" s="17" t="s">
+        <v>265</v>
+      </c>
+      <c r="C18" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="D18" s="19" t="s">
+      <c r="D18" s="17" t="s">
         <v>79</v>
       </c>
-      <c r="E18" s="19" t="s">
-        <v>35</v>
-      </c>
-      <c r="F18" s="19" t="s">
-        <v>76</v>
-      </c>
-      <c r="G18" s="19" t="s">
+      <c r="E18" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="F18" s="17" t="s">
+        <v>76</v>
+      </c>
+      <c r="G18" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="H18" s="19" t="s">
+      <c r="H18" s="17" t="s">
         <v>109</v>
       </c>
-      <c r="I18" s="19" t="s">
-        <v>266</v>
-      </c>
-      <c r="J18" s="20" t="s">
-        <v>267</v>
-      </c>
-      <c r="K18" s="21" t="s">
-        <v>53</v>
-      </c>
-      <c r="L18" s="21" t="s">
-        <v>2</v>
-      </c>
-      <c r="M18" s="19" t="s">
+      <c r="I18" s="17" t="s">
+        <v>266</v>
+      </c>
+      <c r="J18" s="18" t="s">
+        <v>267</v>
+      </c>
+      <c r="K18" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="L18" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="M18" s="17" t="s">
         <v>63</v>
       </c>
-      <c r="N18" s="19" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="19" spans="1:14" s="22" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="19" t="s">
+      <c r="N18" s="17" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="17" t="s">
         <v>158</v>
       </c>
-      <c r="B19" s="19" t="s">
-        <v>265</v>
-      </c>
-      <c r="C19" s="19" t="s">
+      <c r="B19" s="17" t="s">
+        <v>265</v>
+      </c>
+      <c r="C19" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="D19" s="19" t="s">
+      <c r="D19" s="17" t="s">
         <v>79</v>
       </c>
-      <c r="E19" s="19" t="s">
-        <v>35</v>
-      </c>
-      <c r="F19" s="19" t="s">
-        <v>76</v>
-      </c>
-      <c r="G19" s="19" t="s">
+      <c r="E19" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="F19" s="17" t="s">
+        <v>76</v>
+      </c>
+      <c r="G19" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="H19" s="19" t="s">
+      <c r="H19" s="17" t="s">
         <v>118</v>
       </c>
-      <c r="I19" s="19" t="s">
-        <v>266</v>
-      </c>
-      <c r="J19" s="20" t="s">
-        <v>267</v>
-      </c>
-      <c r="K19" s="21" t="s">
-        <v>53</v>
-      </c>
-      <c r="L19" s="21" t="s">
-        <v>2</v>
-      </c>
-      <c r="M19" s="19" t="s">
+      <c r="I19" s="17" t="s">
+        <v>266</v>
+      </c>
+      <c r="J19" s="18" t="s">
+        <v>267</v>
+      </c>
+      <c r="K19" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="L19" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="M19" s="17" t="s">
         <v>62</v>
       </c>
-      <c r="N19" s="19" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="20" spans="1:14" s="22" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="19" t="s">
+      <c r="N19" s="17" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="17" t="s">
         <v>159</v>
       </c>
-      <c r="B20" s="19" t="s">
-        <v>265</v>
-      </c>
-      <c r="C20" s="19" t="s">
+      <c r="B20" s="17" t="s">
+        <v>265</v>
+      </c>
+      <c r="C20" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="D20" s="19" t="s">
+      <c r="D20" s="17" t="s">
         <v>79</v>
       </c>
-      <c r="E20" s="19" t="s">
-        <v>35</v>
-      </c>
-      <c r="F20" s="19" t="s">
-        <v>76</v>
-      </c>
-      <c r="G20" s="19" t="s">
+      <c r="E20" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="F20" s="17" t="s">
+        <v>76</v>
+      </c>
+      <c r="G20" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="H20" s="19" t="s">
+      <c r="H20" s="17" t="s">
         <v>118</v>
       </c>
-      <c r="I20" s="19" t="s">
-        <v>266</v>
-      </c>
-      <c r="J20" s="20" t="s">
-        <v>267</v>
-      </c>
-      <c r="K20" s="21" t="s">
-        <v>53</v>
-      </c>
-      <c r="L20" s="21" t="s">
-        <v>2</v>
-      </c>
-      <c r="M20" s="19" t="s">
+      <c r="I20" s="17" t="s">
+        <v>266</v>
+      </c>
+      <c r="J20" s="18" t="s">
+        <v>267</v>
+      </c>
+      <c r="K20" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="L20" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="M20" s="17" t="s">
         <v>63</v>
       </c>
-      <c r="N20" s="19" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="21" spans="1:14" s="22" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="22" t="s">
+      <c r="N20" s="17" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="20" t="s">
         <v>160</v>
       </c>
-      <c r="B21" s="19" t="s">
-        <v>265</v>
-      </c>
-      <c r="C21" s="19" t="s">
+      <c r="B21" s="17" t="s">
+        <v>265</v>
+      </c>
+      <c r="C21" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="D21" s="22" t="s">
+      <c r="D21" s="20" t="s">
         <v>225</v>
       </c>
-      <c r="E21" s="19" t="s">
-        <v>35</v>
-      </c>
-      <c r="F21" s="19" t="s">
-        <v>76</v>
-      </c>
-      <c r="G21" s="19" t="s">
+      <c r="E21" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="F21" s="17" t="s">
+        <v>76</v>
+      </c>
+      <c r="G21" s="17" t="s">
         <v>236</v>
       </c>
-      <c r="H21" s="22" t="s">
+      <c r="H21" s="20" t="s">
         <v>246</v>
       </c>
-      <c r="I21" s="19" t="s">
-        <v>266</v>
-      </c>
-      <c r="J21" s="20" t="s">
-        <v>267</v>
-      </c>
-      <c r="K21" s="21" t="s">
-        <v>53</v>
-      </c>
-      <c r="L21" s="21" t="s">
-        <v>2</v>
-      </c>
-      <c r="M21" s="22" t="s">
-        <v>2</v>
-      </c>
-      <c r="N21" s="19" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="22" spans="1:14" s="22" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="19" t="s">
+      <c r="I21" s="17" t="s">
+        <v>266</v>
+      </c>
+      <c r="J21" s="18" t="s">
+        <v>267</v>
+      </c>
+      <c r="K21" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="L21" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="M21" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="N21" s="17" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="17" t="s">
         <v>161</v>
       </c>
-      <c r="B22" s="19" t="s">
-        <v>265</v>
-      </c>
-      <c r="C22" s="19" t="s">
+      <c r="B22" s="17" t="s">
+        <v>265</v>
+      </c>
+      <c r="C22" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="D22" s="19" t="s">
+      <c r="D22" s="17" t="s">
         <v>79</v>
       </c>
-      <c r="E22" s="19" t="s">
-        <v>35</v>
-      </c>
-      <c r="F22" s="19" t="s">
-        <v>76</v>
-      </c>
-      <c r="G22" s="19" t="s">
+      <c r="E22" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="F22" s="17" t="s">
+        <v>76</v>
+      </c>
+      <c r="G22" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="H22" s="19" t="s">
+      <c r="H22" s="17" t="s">
         <v>111</v>
       </c>
-      <c r="I22" s="19" t="s">
-        <v>266</v>
-      </c>
-      <c r="J22" s="20" t="s">
-        <v>267</v>
-      </c>
-      <c r="K22" s="21" t="s">
-        <v>53</v>
-      </c>
-      <c r="L22" s="21" t="s">
-        <v>2</v>
-      </c>
-      <c r="M22" s="19" t="s">
+      <c r="I22" s="17" t="s">
+        <v>266</v>
+      </c>
+      <c r="J22" s="18" t="s">
+        <v>267</v>
+      </c>
+      <c r="K22" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="L22" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="M22" s="17" t="s">
         <v>62</v>
       </c>
-      <c r="N22" s="19" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="23" spans="1:14" s="22" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="19" t="s">
+      <c r="N22" s="17" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="17" t="s">
         <v>162</v>
       </c>
-      <c r="B23" s="19" t="s">
-        <v>265</v>
-      </c>
-      <c r="C23" s="19" t="s">
+      <c r="B23" s="17" t="s">
+        <v>265</v>
+      </c>
+      <c r="C23" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="D23" s="19" t="s">
+      <c r="D23" s="17" t="s">
         <v>79</v>
       </c>
-      <c r="E23" s="19" t="s">
-        <v>35</v>
-      </c>
-      <c r="F23" s="19" t="s">
-        <v>76</v>
-      </c>
-      <c r="G23" s="19" t="s">
+      <c r="E23" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="F23" s="17" t="s">
+        <v>76</v>
+      </c>
+      <c r="G23" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="H23" s="19" t="s">
+      <c r="H23" s="17" t="s">
         <v>111</v>
       </c>
-      <c r="I23" s="19" t="s">
-        <v>266</v>
-      </c>
-      <c r="J23" s="20" t="s">
-        <v>267</v>
-      </c>
-      <c r="K23" s="21" t="s">
-        <v>53</v>
-      </c>
-      <c r="L23" s="21" t="s">
-        <v>2</v>
-      </c>
-      <c r="M23" s="19" t="s">
+      <c r="I23" s="17" t="s">
+        <v>266</v>
+      </c>
+      <c r="J23" s="18" t="s">
+        <v>267</v>
+      </c>
+      <c r="K23" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="L23" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="M23" s="17" t="s">
         <v>63</v>
       </c>
-      <c r="N23" s="19" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="24" spans="1:14" s="22" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="22" t="s">
+      <c r="N23" s="17" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="20" t="s">
         <v>163</v>
       </c>
-      <c r="B24" s="19" t="s">
-        <v>265</v>
-      </c>
-      <c r="C24" s="19" t="s">
+      <c r="B24" s="17" t="s">
+        <v>265</v>
+      </c>
+      <c r="C24" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="D24" s="22" t="s">
+      <c r="D24" s="20" t="s">
         <v>225</v>
       </c>
-      <c r="E24" s="19" t="s">
-        <v>35</v>
-      </c>
-      <c r="F24" s="19" t="s">
-        <v>76</v>
-      </c>
-      <c r="G24" s="19" t="s">
+      <c r="E24" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="F24" s="17" t="s">
+        <v>76</v>
+      </c>
+      <c r="G24" s="17" t="s">
         <v>237</v>
       </c>
-      <c r="H24" s="22" t="s">
+      <c r="H24" s="20" t="s">
         <v>247</v>
       </c>
-      <c r="I24" s="19" t="s">
-        <v>266</v>
-      </c>
-      <c r="J24" s="20" t="s">
-        <v>267</v>
-      </c>
-      <c r="K24" s="21" t="s">
-        <v>53</v>
-      </c>
-      <c r="L24" s="21" t="s">
-        <v>2</v>
-      </c>
-      <c r="M24" s="22" t="s">
-        <v>2</v>
-      </c>
-      <c r="N24" s="19" t="s">
+      <c r="I24" s="17" t="s">
+        <v>266</v>
+      </c>
+      <c r="J24" s="18" t="s">
+        <v>267</v>
+      </c>
+      <c r="K24" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="L24" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="M24" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="N24" s="17" t="s">
         <v>55</v>
       </c>
     </row>
@@ -2994,135 +3028,135 @@
         <v>55</v>
       </c>
     </row>
-    <row r="27" spans="1:14" s="22" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="22" t="s">
+    <row r="27" spans="1:14" s="20" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="20" t="s">
         <v>166</v>
       </c>
-      <c r="B27" s="19" t="s">
-        <v>265</v>
-      </c>
-      <c r="C27" s="19" t="s">
+      <c r="B27" s="17" t="s">
+        <v>265</v>
+      </c>
+      <c r="C27" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="D27" s="22" t="s">
+      <c r="D27" s="20" t="s">
         <v>225</v>
       </c>
-      <c r="E27" s="19" t="s">
-        <v>35</v>
-      </c>
-      <c r="F27" s="19" t="s">
-        <v>76</v>
-      </c>
-      <c r="G27" s="19" t="s">
+      <c r="E27" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="F27" s="17" t="s">
+        <v>76</v>
+      </c>
+      <c r="G27" s="17" t="s">
         <v>238</v>
       </c>
-      <c r="H27" s="22" t="s">
+      <c r="H27" s="20" t="s">
         <v>248</v>
       </c>
-      <c r="I27" s="19" t="s">
-        <v>266</v>
-      </c>
-      <c r="J27" s="20" t="s">
-        <v>267</v>
-      </c>
-      <c r="K27" s="21" t="s">
-        <v>53</v>
-      </c>
-      <c r="L27" s="21" t="s">
-        <v>2</v>
-      </c>
-      <c r="M27" s="22" t="s">
-        <v>2</v>
-      </c>
-      <c r="N27" s="19" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="28" spans="1:14" s="22" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="19" t="s">
+      <c r="I27" s="17" t="s">
+        <v>266</v>
+      </c>
+      <c r="J27" s="18" t="s">
+        <v>267</v>
+      </c>
+      <c r="K27" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="L27" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="M27" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="N27" s="17" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" s="20" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="17" t="s">
         <v>167</v>
       </c>
-      <c r="B28" s="19" t="s">
-        <v>265</v>
-      </c>
-      <c r="C28" s="19" t="s">
+      <c r="B28" s="17" t="s">
+        <v>265</v>
+      </c>
+      <c r="C28" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="D28" s="19" t="s">
+      <c r="D28" s="17" t="s">
         <v>79</v>
       </c>
-      <c r="E28" s="19" t="s">
-        <v>35</v>
-      </c>
-      <c r="F28" s="19" t="s">
-        <v>76</v>
-      </c>
-      <c r="G28" s="19" t="s">
+      <c r="E28" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="F28" s="17" t="s">
+        <v>76</v>
+      </c>
+      <c r="G28" s="17" t="s">
         <v>42</v>
       </c>
-      <c r="H28" s="19" t="s">
+      <c r="H28" s="17" t="s">
         <v>113</v>
       </c>
-      <c r="I28" s="19" t="s">
-        <v>266</v>
-      </c>
-      <c r="J28" s="20" t="s">
-        <v>267</v>
-      </c>
-      <c r="K28" s="21" t="s">
-        <v>53</v>
-      </c>
-      <c r="L28" s="21" t="s">
-        <v>2</v>
-      </c>
-      <c r="M28" s="19" t="s">
+      <c r="I28" s="17" t="s">
+        <v>266</v>
+      </c>
+      <c r="J28" s="18" t="s">
+        <v>267</v>
+      </c>
+      <c r="K28" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="L28" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="M28" s="17" t="s">
         <v>62</v>
       </c>
-      <c r="N28" s="19" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="29" spans="1:14" s="22" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="19" t="s">
+      <c r="N28" s="17" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" s="20" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="17" t="s">
         <v>168</v>
       </c>
-      <c r="B29" s="19" t="s">
-        <v>265</v>
-      </c>
-      <c r="C29" s="19" t="s">
+      <c r="B29" s="17" t="s">
+        <v>265</v>
+      </c>
+      <c r="C29" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="D29" s="19" t="s">
+      <c r="D29" s="17" t="s">
         <v>79</v>
       </c>
-      <c r="E29" s="19" t="s">
-        <v>35</v>
-      </c>
-      <c r="F29" s="19" t="s">
-        <v>76</v>
-      </c>
-      <c r="G29" s="19" t="s">
+      <c r="E29" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="F29" s="17" t="s">
+        <v>76</v>
+      </c>
+      <c r="G29" s="17" t="s">
         <v>42</v>
       </c>
-      <c r="H29" s="19" t="s">
+      <c r="H29" s="17" t="s">
         <v>113</v>
       </c>
-      <c r="I29" s="19" t="s">
-        <v>266</v>
-      </c>
-      <c r="J29" s="20" t="s">
-        <v>267</v>
-      </c>
-      <c r="K29" s="21" t="s">
-        <v>53</v>
-      </c>
-      <c r="L29" s="21" t="s">
-        <v>2</v>
-      </c>
-      <c r="M29" s="19" t="s">
+      <c r="I29" s="17" t="s">
+        <v>266</v>
+      </c>
+      <c r="J29" s="18" t="s">
+        <v>267</v>
+      </c>
+      <c r="K29" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="L29" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="M29" s="17" t="s">
         <v>63</v>
       </c>
-      <c r="N29" s="19" t="s">
+      <c r="N29" s="17" t="s">
         <v>55</v>
       </c>
     </row>
@@ -3214,47 +3248,47 @@
         <v>55</v>
       </c>
     </row>
-    <row r="32" spans="1:14" s="22" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="22" t="s">
+    <row r="32" spans="1:14" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="20" t="s">
         <v>171</v>
       </c>
-      <c r="B32" s="19" t="s">
-        <v>265</v>
-      </c>
-      <c r="C32" s="19" t="s">
+      <c r="B32" s="17" t="s">
+        <v>265</v>
+      </c>
+      <c r="C32" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="D32" s="22" t="s">
+      <c r="D32" s="20" t="s">
         <v>225</v>
       </c>
-      <c r="E32" s="19" t="s">
-        <v>35</v>
-      </c>
-      <c r="F32" s="19" t="s">
-        <v>76</v>
-      </c>
-      <c r="G32" s="19" t="s">
+      <c r="E32" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="F32" s="17" t="s">
+        <v>76</v>
+      </c>
+      <c r="G32" s="17" t="s">
         <v>239</v>
       </c>
-      <c r="H32" s="22" t="s">
+      <c r="H32" s="20" t="s">
         <v>249</v>
       </c>
-      <c r="I32" s="19" t="s">
-        <v>266</v>
-      </c>
-      <c r="J32" s="20" t="s">
-        <v>267</v>
-      </c>
-      <c r="K32" s="21" t="s">
+      <c r="I32" s="17" t="s">
+        <v>266</v>
+      </c>
+      <c r="J32" s="18" t="s">
+        <v>267</v>
+      </c>
+      <c r="K32" s="19" t="s">
         <v>59</v>
       </c>
-      <c r="L32" s="21" t="s">
-        <v>2</v>
-      </c>
-      <c r="M32" s="22" t="s">
-        <v>2</v>
-      </c>
-      <c r="N32" s="19" t="s">
+      <c r="L32" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="M32" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="N32" s="17" t="s">
         <v>55</v>
       </c>
     </row>
@@ -3346,179 +3380,179 @@
         <v>55</v>
       </c>
     </row>
-    <row r="35" spans="1:14" s="22" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="22" t="s">
+    <row r="35" spans="1:14" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="20" t="s">
         <v>174</v>
       </c>
-      <c r="B35" s="19" t="s">
-        <v>265</v>
-      </c>
-      <c r="C35" s="19" t="s">
+      <c r="B35" s="17" t="s">
+        <v>265</v>
+      </c>
+      <c r="C35" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="D35" s="22" t="s">
+      <c r="D35" s="20" t="s">
         <v>225</v>
       </c>
-      <c r="E35" s="19" t="s">
-        <v>35</v>
-      </c>
-      <c r="F35" s="19" t="s">
-        <v>76</v>
-      </c>
-      <c r="G35" s="19" t="s">
+      <c r="E35" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="F35" s="17" t="s">
+        <v>76</v>
+      </c>
+      <c r="G35" s="17" t="s">
         <v>240</v>
       </c>
-      <c r="H35" s="22" t="s">
+      <c r="H35" s="20" t="s">
         <v>250</v>
       </c>
-      <c r="I35" s="19" t="s">
-        <v>266</v>
-      </c>
-      <c r="J35" s="20" t="s">
-        <v>267</v>
-      </c>
-      <c r="K35" s="21" t="s">
-        <v>53</v>
-      </c>
-      <c r="L35" s="21" t="s">
-        <v>2</v>
-      </c>
-      <c r="M35" s="22" t="s">
-        <v>2</v>
-      </c>
-      <c r="N35" s="19" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="36" spans="1:14" s="22" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="19" t="s">
+      <c r="I35" s="17" t="s">
+        <v>266</v>
+      </c>
+      <c r="J35" s="18" t="s">
+        <v>267</v>
+      </c>
+      <c r="K35" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="L35" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="M35" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="N35" s="17" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="17" t="s">
         <v>175</v>
       </c>
-      <c r="B36" s="19" t="s">
-        <v>265</v>
-      </c>
-      <c r="C36" s="19" t="s">
+      <c r="B36" s="17" t="s">
+        <v>265</v>
+      </c>
+      <c r="C36" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="D36" s="19" t="s">
+      <c r="D36" s="17" t="s">
         <v>79</v>
       </c>
-      <c r="E36" s="19" t="s">
-        <v>35</v>
-      </c>
-      <c r="F36" s="19" t="s">
-        <v>76</v>
-      </c>
-      <c r="G36" s="19" t="s">
+      <c r="E36" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="F36" s="17" t="s">
+        <v>76</v>
+      </c>
+      <c r="G36" s="17" t="s">
         <v>47</v>
       </c>
-      <c r="H36" s="19" t="s">
+      <c r="H36" s="17" t="s">
         <v>116</v>
       </c>
-      <c r="I36" s="19" t="s">
-        <v>266</v>
-      </c>
-      <c r="J36" s="20" t="s">
-        <v>267</v>
-      </c>
-      <c r="K36" s="21" t="s">
-        <v>53</v>
-      </c>
-      <c r="L36" s="21" t="s">
-        <v>2</v>
-      </c>
-      <c r="M36" s="19" t="s">
+      <c r="I36" s="17" t="s">
+        <v>266</v>
+      </c>
+      <c r="J36" s="18" t="s">
+        <v>267</v>
+      </c>
+      <c r="K36" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="L36" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="M36" s="17" t="s">
         <v>62</v>
       </c>
-      <c r="N36" s="19" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="37" spans="1:14" s="22" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="19" t="s">
+      <c r="N36" s="17" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="17" t="s">
         <v>176</v>
       </c>
-      <c r="B37" s="19" t="s">
-        <v>265</v>
-      </c>
-      <c r="C37" s="19" t="s">
+      <c r="B37" s="17" t="s">
+        <v>265</v>
+      </c>
+      <c r="C37" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="D37" s="19" t="s">
+      <c r="D37" s="17" t="s">
         <v>79</v>
       </c>
-      <c r="E37" s="19" t="s">
-        <v>35</v>
-      </c>
-      <c r="F37" s="19" t="s">
-        <v>76</v>
-      </c>
-      <c r="G37" s="19" t="s">
+      <c r="E37" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="F37" s="17" t="s">
+        <v>76</v>
+      </c>
+      <c r="G37" s="17" t="s">
         <v>47</v>
       </c>
-      <c r="H37" s="19" t="s">
+      <c r="H37" s="17" t="s">
         <v>116</v>
       </c>
-      <c r="I37" s="19" t="s">
-        <v>266</v>
-      </c>
-      <c r="J37" s="20" t="s">
-        <v>267</v>
-      </c>
-      <c r="K37" s="21" t="s">
-        <v>53</v>
-      </c>
-      <c r="L37" s="21" t="s">
-        <v>2</v>
-      </c>
-      <c r="M37" s="19" t="s">
+      <c r="I37" s="17" t="s">
+        <v>266</v>
+      </c>
+      <c r="J37" s="18" t="s">
+        <v>267</v>
+      </c>
+      <c r="K37" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="L37" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="M37" s="17" t="s">
         <v>63</v>
       </c>
-      <c r="N37" s="19" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="38" spans="1:14" s="22" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="22" t="s">
+      <c r="N37" s="17" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="20" t="s">
         <v>177</v>
       </c>
-      <c r="B38" s="19" t="s">
-        <v>265</v>
-      </c>
-      <c r="C38" s="19" t="s">
+      <c r="B38" s="17" t="s">
+        <v>265</v>
+      </c>
+      <c r="C38" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="D38" s="22" t="s">
+      <c r="D38" s="20" t="s">
         <v>225</v>
       </c>
-      <c r="E38" s="19" t="s">
-        <v>35</v>
-      </c>
-      <c r="F38" s="19" t="s">
-        <v>76</v>
-      </c>
-      <c r="G38" s="19" t="s">
+      <c r="E38" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="F38" s="17" t="s">
+        <v>76</v>
+      </c>
+      <c r="G38" s="17" t="s">
         <v>241</v>
       </c>
-      <c r="H38" s="22" t="s">
+      <c r="H38" s="20" t="s">
         <v>251</v>
       </c>
-      <c r="I38" s="19" t="s">
-        <v>266</v>
-      </c>
-      <c r="J38" s="20" t="s">
-        <v>267</v>
-      </c>
-      <c r="K38" s="21" t="s">
-        <v>53</v>
-      </c>
-      <c r="L38" s="21" t="s">
-        <v>2</v>
-      </c>
-      <c r="M38" s="22" t="s">
-        <v>2</v>
-      </c>
-      <c r="N38" s="19" t="s">
+      <c r="I38" s="17" t="s">
+        <v>266</v>
+      </c>
+      <c r="J38" s="18" t="s">
+        <v>267</v>
+      </c>
+      <c r="K38" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="L38" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="M38" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="N38" s="17" t="s">
         <v>55</v>
       </c>
     </row>
@@ -4314,47 +4348,47 @@
         <v>55</v>
       </c>
     </row>
-    <row r="57" spans="1:14" s="22" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A57" s="19" t="s">
+    <row r="57" spans="1:14" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A57" s="17" t="s">
         <v>253</v>
       </c>
-      <c r="B57" s="19" t="s">
-        <v>265</v>
-      </c>
-      <c r="C57" s="19" t="s">
+      <c r="B57" s="17" t="s">
+        <v>265</v>
+      </c>
+      <c r="C57" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="D57" s="22" t="s">
+      <c r="D57" s="20" t="s">
         <v>225</v>
       </c>
-      <c r="E57" s="19" t="s">
-        <v>35</v>
-      </c>
-      <c r="F57" s="19" t="s">
-        <v>76</v>
-      </c>
-      <c r="G57" s="22" t="s">
+      <c r="E57" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="F57" s="17" t="s">
+        <v>76</v>
+      </c>
+      <c r="G57" s="20" t="s">
         <v>226</v>
       </c>
-      <c r="H57" s="22" t="s">
+      <c r="H57" s="20" t="s">
         <v>227</v>
       </c>
-      <c r="I57" s="19" t="s">
-        <v>266</v>
-      </c>
-      <c r="J57" s="20" t="s">
-        <v>267</v>
-      </c>
-      <c r="K57" s="21" t="s">
+      <c r="I57" s="17" t="s">
+        <v>266</v>
+      </c>
+      <c r="J57" s="18" t="s">
+        <v>267</v>
+      </c>
+      <c r="K57" s="19" t="s">
         <v>59</v>
       </c>
-      <c r="L57" s="21" t="s">
-        <v>2</v>
-      </c>
-      <c r="M57" s="22" t="s">
-        <v>2</v>
-      </c>
-      <c r="N57" s="19" t="s">
+      <c r="L57" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="M57" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="N57" s="17" t="s">
         <v>55</v>
       </c>
     </row>
@@ -4402,91 +4436,91 @@
         <v>55</v>
       </c>
     </row>
-    <row r="59" spans="1:14" s="18" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A59" s="15" t="s">
+    <row r="59" spans="1:14" s="16" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A59" s="13" t="s">
         <v>255</v>
       </c>
-      <c r="B59" s="15" t="s">
+      <c r="B59" s="13" t="s">
         <v>265</v>
       </c>
       <c r="C59" s="11" t="s">
         <v>276</v>
       </c>
-      <c r="D59" s="14" t="s">
+      <c r="D59" s="12" t="s">
         <v>277</v>
       </c>
-      <c r="E59" s="15" t="s">
-        <v>35</v>
-      </c>
-      <c r="F59" s="15" t="s">
-        <v>76</v>
-      </c>
-      <c r="G59" s="15" t="s">
+      <c r="E59" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="F59" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="G59" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="H59" s="15" t="s">
+      <c r="H59" s="13" t="s">
         <v>99</v>
       </c>
-      <c r="I59" s="15" t="s">
-        <v>266</v>
-      </c>
-      <c r="J59" s="16" t="s">
-        <v>267</v>
-      </c>
-      <c r="K59" s="17" t="s">
-        <v>53</v>
-      </c>
-      <c r="L59" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="M59" s="15" t="s">
-        <v>2</v>
-      </c>
-      <c r="N59" s="15" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="60" spans="1:14" s="18" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A60" s="15" t="s">
+      <c r="I59" s="13" t="s">
+        <v>266</v>
+      </c>
+      <c r="J59" s="14" t="s">
+        <v>267</v>
+      </c>
+      <c r="K59" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="L59" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="M59" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="N59" s="13" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="60" spans="1:14" s="16" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A60" s="13" t="s">
         <v>256</v>
       </c>
-      <c r="B60" s="15" t="s">
+      <c r="B60" s="13" t="s">
         <v>265</v>
       </c>
       <c r="C60" s="11" t="s">
         <v>276</v>
       </c>
-      <c r="D60" s="14" t="s">
+      <c r="D60" s="12" t="s">
         <v>277</v>
       </c>
-      <c r="E60" s="15" t="s">
-        <v>35</v>
-      </c>
-      <c r="F60" s="15" t="s">
-        <v>76</v>
-      </c>
-      <c r="G60" s="15" t="s">
+      <c r="E60" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="F60" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="G60" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="H60" s="15" t="s">
+      <c r="H60" s="13" t="s">
         <v>106</v>
       </c>
-      <c r="I60" s="15" t="s">
-        <v>266</v>
-      </c>
-      <c r="J60" s="16" t="s">
-        <v>2</v>
-      </c>
-      <c r="K60" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="L60" s="17" t="s">
+      <c r="I60" s="13" t="s">
+        <v>266</v>
+      </c>
+      <c r="J60" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="K60" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="L60" s="15" t="s">
         <v>56</v>
       </c>
-      <c r="M60" s="15" t="s">
-        <v>2</v>
-      </c>
-      <c r="N60" s="15" t="s">
+      <c r="M60" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="N60" s="13" t="s">
         <v>55</v>
       </c>
     </row>
@@ -5018,47 +5052,47 @@
         <v>55</v>
       </c>
     </row>
-    <row r="73" spans="1:14" s="22" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A73" s="22" t="s">
+    <row r="73" spans="1:14" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A73" s="20" t="s">
         <v>207</v>
       </c>
-      <c r="B73" s="19" t="s">
-        <v>265</v>
-      </c>
-      <c r="C73" s="19" t="s">
+      <c r="B73" s="17" t="s">
+        <v>265</v>
+      </c>
+      <c r="C73" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="D73" s="22" t="s">
+      <c r="D73" s="20" t="s">
         <v>225</v>
       </c>
-      <c r="E73" s="19" t="s">
-        <v>35</v>
-      </c>
-      <c r="F73" s="19" t="s">
-        <v>76</v>
-      </c>
-      <c r="G73" s="22" t="s">
+      <c r="E73" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="F73" s="17" t="s">
+        <v>76</v>
+      </c>
+      <c r="G73" s="20" t="s">
         <v>228</v>
       </c>
-      <c r="H73" s="22" t="s">
+      <c r="H73" s="20" t="s">
         <v>229</v>
       </c>
-      <c r="I73" s="19" t="s">
-        <v>266</v>
-      </c>
-      <c r="J73" s="20" t="s">
-        <v>267</v>
-      </c>
-      <c r="K73" s="21" t="s">
-        <v>53</v>
-      </c>
-      <c r="L73" s="21" t="s">
-        <v>2</v>
-      </c>
-      <c r="M73" s="22" t="s">
-        <v>2</v>
-      </c>
-      <c r="N73" s="19" t="s">
+      <c r="I73" s="17" t="s">
+        <v>266</v>
+      </c>
+      <c r="J73" s="18" t="s">
+        <v>267</v>
+      </c>
+      <c r="K73" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="L73" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="M73" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="N73" s="17" t="s">
         <v>55</v>
       </c>
     </row>
@@ -5678,47 +5712,47 @@
         <v>55</v>
       </c>
     </row>
-    <row r="88" spans="1:14" s="22" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A88" s="22" t="s">
+    <row r="88" spans="1:14" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A88" s="20" t="s">
         <v>222</v>
       </c>
-      <c r="B88" s="19" t="s">
-        <v>265</v>
-      </c>
-      <c r="C88" s="19" t="s">
+      <c r="B88" s="17" t="s">
+        <v>265</v>
+      </c>
+      <c r="C88" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="D88" s="22" t="s">
+      <c r="D88" s="20" t="s">
         <v>225</v>
       </c>
-      <c r="E88" s="19" t="s">
-        <v>35</v>
-      </c>
-      <c r="F88" s="19" t="s">
-        <v>76</v>
-      </c>
-      <c r="G88" s="22" t="s">
+      <c r="E88" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="F88" s="17" t="s">
+        <v>76</v>
+      </c>
+      <c r="G88" s="20" t="s">
         <v>230</v>
       </c>
-      <c r="H88" s="22" t="s">
+      <c r="H88" s="20" t="s">
         <v>231</v>
       </c>
-      <c r="I88" s="19" t="s">
-        <v>266</v>
-      </c>
-      <c r="J88" s="20" t="s">
-        <v>267</v>
-      </c>
-      <c r="K88" s="21" t="s">
+      <c r="I88" s="17" t="s">
+        <v>266</v>
+      </c>
+      <c r="J88" s="18" t="s">
+        <v>267</v>
+      </c>
+      <c r="K88" s="19" t="s">
         <v>70</v>
       </c>
-      <c r="L88" s="21" t="s">
-        <v>2</v>
-      </c>
-      <c r="M88" s="22" t="s">
-        <v>2</v>
-      </c>
-      <c r="N88" s="19" t="s">
+      <c r="L88" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="M88" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="N88" s="17" t="s">
         <v>55</v>
       </c>
     </row>
@@ -5854,443 +5888,443 @@
         <v>55</v>
       </c>
     </row>
-    <row r="92" spans="1:14" s="11" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A92" s="11" t="s">
+    <row r="92" spans="1:14" s="28" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A92" s="28" t="s">
         <v>268</v>
       </c>
-      <c r="B92" s="12" t="s">
-        <v>265</v>
-      </c>
-      <c r="C92" s="11" t="s">
+      <c r="B92" s="29" t="s">
+        <v>265</v>
+      </c>
+      <c r="C92" s="28" t="s">
         <v>276</v>
       </c>
-      <c r="D92" s="14" t="s">
+      <c r="D92" s="30" t="s">
         <v>277</v>
       </c>
-      <c r="E92" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="F92" s="12" t="s">
-        <v>76</v>
-      </c>
-      <c r="G92" s="15" t="s">
+      <c r="E92" s="28" t="s">
+        <v>35</v>
+      </c>
+      <c r="F92" s="29" t="s">
+        <v>76</v>
+      </c>
+      <c r="G92" s="29" t="s">
         <v>19</v>
       </c>
-      <c r="H92" s="15" t="s">
+      <c r="H92" s="29" t="s">
         <v>99</v>
       </c>
-      <c r="I92" s="12" t="s">
-        <v>266</v>
-      </c>
-      <c r="J92" s="14" t="s">
-        <v>267</v>
-      </c>
-      <c r="K92" s="13" t="s">
-        <v>53</v>
-      </c>
-      <c r="L92" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="M92" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="N92" s="12" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="93" spans="1:14" s="11" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A93" s="24" t="s">
+      <c r="I92" s="29" t="s">
+        <v>266</v>
+      </c>
+      <c r="J92" s="30" t="s">
+        <v>267</v>
+      </c>
+      <c r="K92" s="31" t="s">
+        <v>53</v>
+      </c>
+      <c r="L92" s="31" t="s">
+        <v>2</v>
+      </c>
+      <c r="M92" s="29" t="s">
+        <v>2</v>
+      </c>
+      <c r="N92" s="29" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="93" spans="1:14" s="21" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A93" s="21" t="s">
         <v>269</v>
       </c>
-      <c r="B93" s="25" t="s">
-        <v>265</v>
-      </c>
-      <c r="C93" s="25" t="s">
+      <c r="B93" s="22" t="s">
+        <v>265</v>
+      </c>
+      <c r="C93" s="22" t="s">
         <v>122</v>
       </c>
-      <c r="D93" s="25" t="s">
+      <c r="D93" s="22" t="s">
         <v>123</v>
       </c>
-      <c r="E93" s="25" t="s">
-        <v>35</v>
-      </c>
-      <c r="F93" s="25" t="s">
-        <v>76</v>
-      </c>
-      <c r="G93" s="25" t="s">
+      <c r="E93" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="F93" s="22" t="s">
+        <v>76</v>
+      </c>
+      <c r="G93" s="22" t="s">
         <v>278</v>
       </c>
-      <c r="H93" s="25" t="s">
+      <c r="H93" s="22" t="s">
         <v>279</v>
       </c>
-      <c r="I93" s="25" t="s">
-        <v>266</v>
-      </c>
-      <c r="J93" s="26" t="s">
-        <v>267</v>
-      </c>
-      <c r="K93" s="27" t="s">
-        <v>53</v>
-      </c>
-      <c r="L93" s="27" t="s">
-        <v>2</v>
-      </c>
-      <c r="M93" s="24" t="s">
+      <c r="I93" s="22" t="s">
+        <v>266</v>
+      </c>
+      <c r="J93" s="23" t="s">
+        <v>267</v>
+      </c>
+      <c r="K93" s="24" t="s">
+        <v>53</v>
+      </c>
+      <c r="L93" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="M93" s="21" t="s">
         <v>68</v>
       </c>
-      <c r="N93" s="25" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="94" spans="1:14" s="11" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A94" s="11" t="s">
+      <c r="N93" s="22" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="94" spans="1:14" s="21" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A94" s="21" t="s">
         <v>270</v>
       </c>
-      <c r="B94" s="12" t="s">
-        <v>265</v>
-      </c>
-      <c r="C94" s="12" t="s">
+      <c r="B94" s="22" t="s">
+        <v>265</v>
+      </c>
+      <c r="C94" s="22" t="s">
         <v>122</v>
       </c>
-      <c r="D94" s="12" t="s">
+      <c r="D94" s="22" t="s">
         <v>123</v>
       </c>
-      <c r="E94" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="F94" s="12" t="s">
-        <v>76</v>
-      </c>
-      <c r="G94" s="12" t="s">
-        <v>39</v>
-      </c>
-      <c r="H94" s="12" t="s">
-        <v>103</v>
-      </c>
-      <c r="I94" s="12" t="s">
-        <v>266</v>
-      </c>
-      <c r="J94" s="14" t="s">
-        <v>267</v>
-      </c>
-      <c r="K94" s="13" t="s">
-        <v>53</v>
-      </c>
-      <c r="L94" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="M94" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="N94" s="12" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="95" spans="1:14" s="11" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A95" s="11" t="s">
+      <c r="E94" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="F94" s="22" t="s">
+        <v>76</v>
+      </c>
+      <c r="G94" s="22" t="s">
+        <v>278</v>
+      </c>
+      <c r="H94" s="22" t="s">
+        <v>279</v>
+      </c>
+      <c r="I94" s="22" t="s">
+        <v>266</v>
+      </c>
+      <c r="J94" s="23" t="s">
+        <v>267</v>
+      </c>
+      <c r="K94" s="24" t="s">
+        <v>53</v>
+      </c>
+      <c r="L94" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="M94" s="22" t="s">
+        <v>67</v>
+      </c>
+      <c r="N94" s="22" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="95" spans="1:14" s="28" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A95" s="28" t="s">
         <v>271</v>
       </c>
-      <c r="B95" s="12" t="s">
-        <v>265</v>
-      </c>
-      <c r="C95" s="12" t="s">
+      <c r="B95" s="29" t="s">
+        <v>265</v>
+      </c>
+      <c r="C95" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="D95" s="12" t="s">
+      <c r="D95" s="29" t="s">
         <v>79</v>
       </c>
-      <c r="E95" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="F95" s="12" t="s">
-        <v>76</v>
-      </c>
-      <c r="G95" s="11" t="s">
+      <c r="E95" s="29" t="s">
+        <v>35</v>
+      </c>
+      <c r="F95" s="29" t="s">
+        <v>76</v>
+      </c>
+      <c r="G95" s="28" t="s">
         <v>230</v>
       </c>
-      <c r="H95" s="11" t="s">
+      <c r="H95" s="28" t="s">
         <v>231</v>
       </c>
-      <c r="I95" s="12" t="s">
-        <v>266</v>
-      </c>
-      <c r="J95" s="14" t="s">
-        <v>267</v>
-      </c>
-      <c r="K95" s="13" t="s">
-        <v>53</v>
-      </c>
-      <c r="L95" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="M95" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="N95" s="12" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="96" spans="1:14" s="11" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A96" s="11" t="s">
+      <c r="I95" s="29" t="s">
+        <v>266</v>
+      </c>
+      <c r="J95" s="30" t="s">
+        <v>267</v>
+      </c>
+      <c r="K95" s="31" t="s">
+        <v>53</v>
+      </c>
+      <c r="L95" s="31" t="s">
+        <v>2</v>
+      </c>
+      <c r="M95" s="29" t="s">
+        <v>2</v>
+      </c>
+      <c r="N95" s="29" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="96" spans="1:14" s="28" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A96" s="28" t="s">
         <v>272</v>
       </c>
-      <c r="B96" s="12" t="s">
-        <v>265</v>
-      </c>
-      <c r="C96" s="12" t="s">
+      <c r="B96" s="29" t="s">
+        <v>265</v>
+      </c>
+      <c r="C96" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="D96" s="12" t="s">
+      <c r="D96" s="29" t="s">
         <v>79</v>
       </c>
-      <c r="E96" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="F96" s="12" t="s">
-        <v>76</v>
-      </c>
-      <c r="G96" s="11" t="s">
+      <c r="E96" s="29" t="s">
+        <v>35</v>
+      </c>
+      <c r="F96" s="29" t="s">
+        <v>76</v>
+      </c>
+      <c r="G96" s="28" t="s">
         <v>230</v>
       </c>
-      <c r="H96" s="11" t="s">
+      <c r="H96" s="28" t="s">
         <v>231</v>
       </c>
-      <c r="I96" s="12" t="s">
-        <v>266</v>
-      </c>
-      <c r="J96" s="14" t="s">
-        <v>267</v>
-      </c>
-      <c r="K96" s="13" t="s">
-        <v>53</v>
-      </c>
-      <c r="L96" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="M96" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="N96" s="12" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="97" spans="1:14" s="11" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A97" s="11" t="s">
+      <c r="I96" s="29" t="s">
+        <v>266</v>
+      </c>
+      <c r="J96" s="30" t="s">
+        <v>267</v>
+      </c>
+      <c r="K96" s="31" t="s">
+        <v>53</v>
+      </c>
+      <c r="L96" s="31" t="s">
+        <v>2</v>
+      </c>
+      <c r="M96" s="29" t="s">
+        <v>2</v>
+      </c>
+      <c r="N96" s="29" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="97" spans="1:14" s="21" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A97" s="21" t="s">
         <v>273</v>
       </c>
-      <c r="B97" s="12" t="s">
-        <v>265</v>
-      </c>
-      <c r="C97" s="12" t="s">
+      <c r="B97" s="22" t="s">
+        <v>265</v>
+      </c>
+      <c r="C97" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="D97" s="12" t="s">
+      <c r="D97" s="22" t="s">
         <v>79</v>
       </c>
-      <c r="E97" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="F97" s="12" t="s">
-        <v>76</v>
-      </c>
-      <c r="G97" s="12" t="s">
-        <v>37</v>
-      </c>
-      <c r="H97" s="12" t="s">
-        <v>112</v>
-      </c>
-      <c r="I97" s="12" t="s">
-        <v>266</v>
-      </c>
-      <c r="J97" s="14" t="s">
-        <v>267</v>
-      </c>
-      <c r="K97" s="13" t="s">
-        <v>53</v>
-      </c>
-      <c r="L97" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="M97" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="N97" s="12" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="98" spans="1:14" s="11" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A98" s="11" t="s">
+      <c r="E97" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="F97" s="22" t="s">
+        <v>76</v>
+      </c>
+      <c r="G97" s="25" t="s">
+        <v>280</v>
+      </c>
+      <c r="H97" s="25" t="s">
+        <v>281</v>
+      </c>
+      <c r="I97" s="22" t="s">
+        <v>266</v>
+      </c>
+      <c r="J97" s="23" t="s">
+        <v>267</v>
+      </c>
+      <c r="K97" s="24" t="s">
+        <v>53</v>
+      </c>
+      <c r="L97" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="M97" s="22" t="s">
+        <v>130</v>
+      </c>
+      <c r="N97" s="22" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="98" spans="1:14" s="21" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A98" s="21" t="s">
         <v>274</v>
       </c>
-      <c r="B98" s="12" t="s">
-        <v>265</v>
-      </c>
-      <c r="C98" s="12" t="s">
+      <c r="B98" s="22" t="s">
+        <v>265</v>
+      </c>
+      <c r="C98" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="D98" s="12" t="s">
+      <c r="D98" s="22" t="s">
         <v>79</v>
       </c>
-      <c r="E98" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="F98" s="12" t="s">
-        <v>76</v>
-      </c>
-      <c r="G98" s="12" t="s">
-        <v>37</v>
-      </c>
-      <c r="H98" s="12" t="s">
-        <v>112</v>
-      </c>
-      <c r="I98" s="12" t="s">
-        <v>266</v>
-      </c>
-      <c r="J98" s="14" t="s">
-        <v>267</v>
-      </c>
-      <c r="K98" s="13" t="s">
-        <v>53</v>
-      </c>
-      <c r="L98" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="M98" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="N98" s="12" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="99" spans="1:14" s="11" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A99" s="11" t="s">
+      <c r="E98" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="F98" s="22" t="s">
+        <v>76</v>
+      </c>
+      <c r="G98" s="25" t="s">
+        <v>280</v>
+      </c>
+      <c r="H98" s="25" t="s">
+        <v>281</v>
+      </c>
+      <c r="I98" s="22" t="s">
+        <v>266</v>
+      </c>
+      <c r="J98" s="23" t="s">
+        <v>267</v>
+      </c>
+      <c r="K98" s="24" t="s">
+        <v>53</v>
+      </c>
+      <c r="L98" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="M98" s="22" t="s">
+        <v>129</v>
+      </c>
+      <c r="N98" s="22" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="99" spans="1:14" s="21" customFormat="1" ht="153" x14ac:dyDescent="0.2">
+      <c r="A99" s="21" t="s">
         <v>275</v>
       </c>
-      <c r="B99" s="12" t="s">
-        <v>265</v>
-      </c>
-      <c r="C99" s="12" t="s">
+      <c r="B99" s="22" t="s">
+        <v>265</v>
+      </c>
+      <c r="C99" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="D99" s="11" t="s">
+      <c r="D99" s="21" t="s">
         <v>225</v>
       </c>
-      <c r="E99" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="F99" s="12" t="s">
-        <v>76</v>
-      </c>
-      <c r="G99" s="11" t="s">
-        <v>230</v>
-      </c>
-      <c r="H99" s="11" t="s">
-        <v>231</v>
-      </c>
-      <c r="I99" s="12" t="s">
-        <v>266</v>
-      </c>
-      <c r="J99" s="14" t="s">
-        <v>267</v>
-      </c>
-      <c r="K99" s="13" t="s">
-        <v>53</v>
-      </c>
-      <c r="L99" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="M99" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="N99" s="12" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="100" spans="1:14" s="11" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A100" s="11" t="s">
+      <c r="E99" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="F99" s="22" t="s">
+        <v>76</v>
+      </c>
+      <c r="G99" s="26" t="s">
+        <v>282</v>
+      </c>
+      <c r="H99" s="26" t="s">
+        <v>283</v>
+      </c>
+      <c r="I99" s="22" t="s">
+        <v>266</v>
+      </c>
+      <c r="J99" s="23" t="s">
+        <v>267</v>
+      </c>
+      <c r="K99" s="24" t="s">
+        <v>53</v>
+      </c>
+      <c r="L99" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="M99" s="22" t="s">
+        <v>130</v>
+      </c>
+      <c r="N99" s="22" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="100" spans="1:14" s="21" customFormat="1" ht="68" x14ac:dyDescent="0.2">
+      <c r="A100" s="21" t="s">
         <v>165</v>
       </c>
-      <c r="B100" s="12" t="s">
-        <v>265</v>
-      </c>
-      <c r="C100" s="12" t="s">
+      <c r="B100" s="22" t="s">
+        <v>265</v>
+      </c>
+      <c r="C100" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="D100" s="12" t="s">
+      <c r="D100" s="22" t="s">
         <v>79</v>
       </c>
-      <c r="E100" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="F100" s="12" t="s">
-        <v>76</v>
-      </c>
-      <c r="G100" s="23" t="s">
-        <v>37</v>
-      </c>
-      <c r="H100" s="12" t="s">
-        <v>112</v>
-      </c>
-      <c r="I100" s="12" t="s">
-        <v>266</v>
-      </c>
-      <c r="J100" s="14" t="s">
-        <v>267</v>
-      </c>
-      <c r="K100" s="13" t="s">
-        <v>53</v>
-      </c>
-      <c r="L100" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="M100" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="N100" s="12" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="101" spans="1:14" s="11" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A101" s="11" t="s">
+      <c r="E100" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="F100" s="22" t="s">
+        <v>76</v>
+      </c>
+      <c r="G100" s="27" t="s">
+        <v>284</v>
+      </c>
+      <c r="H100" s="25" t="s">
+        <v>285</v>
+      </c>
+      <c r="I100" s="22" t="s">
+        <v>266</v>
+      </c>
+      <c r="J100" s="23" t="s">
+        <v>267</v>
+      </c>
+      <c r="K100" s="24" t="s">
+        <v>53</v>
+      </c>
+      <c r="L100" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="M100" s="22" t="s">
+        <v>130</v>
+      </c>
+      <c r="N100" s="22" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="101" spans="1:14" s="21" customFormat="1" ht="68" x14ac:dyDescent="0.2">
+      <c r="A101" s="21" t="s">
         <v>164</v>
       </c>
-      <c r="B101" s="12" t="s">
-        <v>265</v>
-      </c>
-      <c r="C101" s="12" t="s">
+      <c r="B101" s="22" t="s">
+        <v>265</v>
+      </c>
+      <c r="C101" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="D101" s="12" t="s">
+      <c r="D101" s="22" t="s">
         <v>79</v>
       </c>
-      <c r="E101" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="F101" s="12" t="s">
-        <v>76</v>
-      </c>
-      <c r="G101" s="23" t="s">
-        <v>37</v>
-      </c>
-      <c r="H101" s="12" t="s">
-        <v>112</v>
-      </c>
-      <c r="I101" s="12" t="s">
-        <v>266</v>
-      </c>
-      <c r="J101" s="14" t="s">
-        <v>267</v>
-      </c>
-      <c r="K101" s="13" t="s">
-        <v>53</v>
-      </c>
-      <c r="L101" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="M101" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="N101" s="12" t="s">
+      <c r="E101" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="F101" s="22" t="s">
+        <v>76</v>
+      </c>
+      <c r="G101" s="27" t="s">
+        <v>284</v>
+      </c>
+      <c r="H101" s="25" t="s">
+        <v>285</v>
+      </c>
+      <c r="I101" s="22" t="s">
+        <v>266</v>
+      </c>
+      <c r="J101" s="23" t="s">
+        <v>267</v>
+      </c>
+      <c r="K101" s="24" t="s">
+        <v>53</v>
+      </c>
+      <c r="L101" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="M101" s="22" t="s">
+        <v>129</v>
+      </c>
+      <c r="N101" s="22" t="s">
         <v>55</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fix disagg for HTS_TST.ActiveOther.Pos
- fix disagg for HTS_TST.ActiveOther.Pos, changed from OtherMod/Age Aggregated/Sex/Result to OtherMod/Age/Sex/Result
</commit_message>
<xml_diff>
--- a/data-raw/snu_x_im_distribution_configuration/23Tto24TMap.xlsx
+++ b/data-raw/snu_x_im_distribution_configuration/23Tto24TMap.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/faustolopezbao/Documents/GitHub/data-pack-commons/data-raw/snu_x_im_distribution_configuration/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{81DFC993-7113-534A-B18A-3BDA55AB6D79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{08C34B0A-7808-104E-BAB4-1821F7A48D1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="36060" yWindow="1040" windowWidth="37520" windowHeight="18980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2700" yWindow="960" windowWidth="30120" windowHeight="18980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Map" sheetId="1" r:id="rId1"/>
@@ -878,12 +878,6 @@
     <t>zzNslrLngKi;xds87opkbem</t>
   </si>
   <si>
-    <t>OtherMod/Age Aggregated/Sex/Result;MobileMod/Age/Sex/Result</t>
-  </si>
-  <si>
-    <t>cYRowDkVEpl;Qr9eyrVLHSg</t>
-  </si>
-  <si>
     <t>IndexMod/Age/Sex/HIVStatus;Index/Age/Sex/HIVStatus;Emergency Ward/Age/Sex/HIVStatus;Inpat/Age/Sex/HIVStatus;MobileMod/Age/Sex/HIVStatus;OtherMod/Age/Sex/HIVStatus;OtherPITC/Age/Sex/HIVStatus;PMTCT PostANC/Age/Sex/HIVStatus;STI Clinic/Age/Sex/HIVStatus;VCT/Age/Sex/HIVStatus;KeyPop/HIVStatus;PMTCT ANC/Age/Sex/HIVStatus;TBClinic/Age/Sex/HIVStatus;VMMC/Age/Sex/HIVStatus</t>
   </si>
   <si>
@@ -894,6 +888,12 @@
   </si>
   <si>
     <t>p6j1mfN4rjP;iPfNX6Ylqp1;E3VaSq4JOzd;dcaYk7TXk4E;iFlQUEQcsfZ;jEpJPF6IVVB</t>
+  </si>
+  <si>
+    <t>OtherMod/Age/Sex/Result;MobileMod/Age/Sex/Result</t>
+  </si>
+  <si>
+    <t>Lhk8mjk6Yk2;Qr9eyrVLHSg</t>
   </si>
 </sst>
 </file>
@@ -1860,9 +1860,9 @@
 <worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N101"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A85" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G99" sqref="G99"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="152" zoomScaleNormal="152" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A87" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H98" sqref="H98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6108,7 +6108,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="97" spans="1:14" s="21" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:14" s="21" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A97" s="21" t="s">
         <v>273</v>
       </c>
@@ -6128,10 +6128,10 @@
         <v>76</v>
       </c>
       <c r="G97" s="25" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
       <c r="H97" s="25" t="s">
-        <v>281</v>
+        <v>285</v>
       </c>
       <c r="I97" s="22" t="s">
         <v>266</v>
@@ -6152,7 +6152,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="98" spans="1:14" s="21" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:14" s="21" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A98" s="21" t="s">
         <v>274</v>
       </c>
@@ -6172,10 +6172,10 @@
         <v>76</v>
       </c>
       <c r="G98" s="25" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
       <c r="H98" s="25" t="s">
-        <v>281</v>
+        <v>285</v>
       </c>
       <c r="I98" s="22" t="s">
         <v>266</v>
@@ -6216,10 +6216,10 @@
         <v>76</v>
       </c>
       <c r="G99" s="26" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="H99" s="26" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="I99" s="22" t="s">
         <v>266</v>
@@ -6260,10 +6260,10 @@
         <v>76</v>
       </c>
       <c r="G100" s="27" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="H100" s="25" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="I100" s="22" t="s">
         <v>266</v>
@@ -6304,10 +6304,10 @@
         <v>76</v>
       </c>
       <c r="G101" s="27" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="H101" s="25" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="I101" s="22" t="s">
         <v>266</v>

</xml_diff>

<commit_message>
add sns to hts_recent
- added new sns data from prod to hts_recent
</commit_message>
<xml_diff>
--- a/data-raw/snu_x_im_distribution_configuration/23Tto24TMap.xlsx
+++ b/data-raw/snu_x_im_distribution_configuration/23Tto24TMap.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/faustolopezbao/Documents/GitHub/data-pack-commons/data-raw/snu_x_im_distribution_configuration/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{B2CDB35A-281D-A94F-871B-6D9DC389D6E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{96D130E4-4264-B644-9510-73EEFFD6DCA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="37580" yWindow="1080" windowWidth="30120" windowHeight="18980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="24260" windowHeight="20400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Map" sheetId="1" r:id="rId1"/>
@@ -884,10 +884,10 @@
     <t>Lhk8mjk6Yk2;Qr9eyrVLHSg</t>
   </si>
   <si>
-    <t>cnlEjFkl5UZ;Tpc0Ztxae9H;lJQyt3PjrVy;CEcYYCkTncR;EVwSAwSEfTg;G6QgzwFMWSP;Y3aCLwI6IU3;c60fuhOWPu4;WGV3YTTqrZ3;vYZLPZAuv8A;FazeYvGkStI;PcsTdqSq0Id;mCtbMQYjHjj</t>
-  </si>
-  <si>
-    <t>IndexMod/Age/Sex/HIVStatus;Index/Age/Sex/HIVStatus;Emergency Ward/Age/Sex/HIVStatus;Inpat/Age/Sex/HIVStatus;MobileMod/Age/Sex/HIVStatus;OtherMod/Age/Sex/HIVStatus;OtherPITC/Age/Sex/HIVStatus;PMTCT PostANC/Age/Sex/HIVStatus;STI Clinic/Age/Sex/HIVStatus;VCT/Age/Sex/HIVStatus;PMTCT ANC/Age/Sex/HIVStatus;TBClinic/Age/Sex/HIVStatus;VMMC/Age/Sex/HIVStatus</t>
+    <t>IndexMod/Age/Sex/HIVStatus;Index/Age/Sex/HIVStatus;Emergency Ward/Age/Sex/HIVStatus;Inpat/Age/Sex/HIVStatus;MobileMod/Age/Sex/HIVStatus;OtherMod/Age/Sex/HIVStatus;OtherPITC/Age/Sex/HIVStatus;PMTCT PostANC/Age/Sex/HIVStatus;STI Clinic/Age/Sex/HIVStatus;VCT/Age/Sex/HIVStatus;PMTCT ANC/Age/Sex/HIVStatus;TBClinic/Age/Sex/HIVStatus;VMMC/Age/Sex/HIVStatus;SNSMod/Age/Sex/HIVStatus;SNS/Age/Sex/HIVStatus</t>
+  </si>
+  <si>
+    <t>cnlEjFkl5UZ;Tpc0Ztxae9H;lJQyt3PjrVy;CEcYYCkTncR;EVwSAwSEfTg;G6QgzwFMWSP;Y3aCLwI6IU3;c60fuhOWPu4;WGV3YTTqrZ3;vYZLPZAuv8A;FazeYvGkStI;PcsTdqSq0Id;mCtbMQYjHjj;ibJUfCOgjxa;icVEv3fDvfA</t>
   </si>
 </sst>
 </file>
@@ -1856,7 +1856,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="111" zoomScaleNormal="111" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A78" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B86" sqref="B86"/>
+      <selection pane="bottomLeft" activeCell="H97" sqref="H97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6102,7 +6102,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="97" spans="1:14" s="21" customFormat="1" ht="136" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:14" s="21" customFormat="1" ht="153" x14ac:dyDescent="0.2">
       <c r="A97" s="21" t="s">
         <v>273</v>
       </c>
@@ -6122,10 +6122,10 @@
         <v>75</v>
       </c>
       <c r="G97" s="26" t="s">
+        <v>282</v>
+      </c>
+      <c r="H97" s="26" t="s">
         <v>283</v>
-      </c>
-      <c r="H97" s="26" t="s">
-        <v>282</v>
       </c>
       <c r="I97" s="22" t="s">
         <v>264</v>

</xml_diff>

<commit_message>
added hts_tst.sns.Pos.T and neg
adding hts_tst.sns.pos.t and neg disagg type etc
</commit_message>
<xml_diff>
--- a/data-raw/snu_x_im_distribution_configuration/23Tto24TMap.xlsx
+++ b/data-raw/snu_x_im_distribution_configuration/23Tto24TMap.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/faustolopezbao/Documents/GitHub/data-pack-commons/data-raw/snu_x_im_distribution_configuration/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{96D130E4-4264-B644-9510-73EEFFD6DCA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{6FE4D896-76E6-D840-B3A6-650B773DA9FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="24260" windowHeight="20400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33820" windowHeight="20520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Map" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="1386" uniqueCount="284">
+<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="1386" uniqueCount="286">
   <si>
     <t>CXCA_SCRN</t>
   </si>
@@ -888,13 +888,19 @@
   </si>
   <si>
     <t>cnlEjFkl5UZ;Tpc0Ztxae9H;lJQyt3PjrVy;CEcYYCkTncR;EVwSAwSEfTg;G6QgzwFMWSP;Y3aCLwI6IU3;c60fuhOWPu4;WGV3YTTqrZ3;vYZLPZAuv8A;FazeYvGkStI;PcsTdqSq0Id;mCtbMQYjHjj;ibJUfCOgjxa;icVEv3fDvfA</t>
+  </si>
+  <si>
+    <t>SNS/Age/Sex/Result;SNSMod/Age/Sex/Result</t>
+  </si>
+  <si>
+    <t>STGTOMk0tLf;BAyV276wNJj</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="22" x14ac:knownFonts="1">
+  <fonts count="23" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1050,6 +1056,12 @@
       <sz val="13"/>
       <color rgb="FF202124"/>
       <name val="Roboto"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="38">
@@ -1449,7 +1461,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1488,6 +1500,7 @@
     <xf numFmtId="0" fontId="19" fillId="37" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="37" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="19" fillId="37" borderId="10" xfId="6" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1855,8 +1868,8 @@
   <dimension ref="A1:N99"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="111" zoomScaleNormal="111" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A78" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H97" sqref="H97"/>
+      <pane ySplit="1" topLeftCell="A74" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H94" sqref="H94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5945,11 +5958,11 @@
       <c r="F93" s="29" t="s">
         <v>75</v>
       </c>
-      <c r="G93" s="28" t="s">
-        <v>228</v>
+      <c r="G93" s="32" t="s">
+        <v>284</v>
       </c>
       <c r="H93" s="28" t="s">
-        <v>229</v>
+        <v>285</v>
       </c>
       <c r="I93" s="29" t="s">
         <v>264</v>
@@ -5964,7 +5977,7 @@
         <v>2</v>
       </c>
       <c r="M93" s="29" t="s">
-        <v>2</v>
+        <v>128</v>
       </c>
       <c r="N93" s="29" t="s">
         <v>54</v>
@@ -5989,11 +6002,11 @@
       <c r="F94" s="29" t="s">
         <v>75</v>
       </c>
-      <c r="G94" s="28" t="s">
-        <v>228</v>
+      <c r="G94" s="32" t="s">
+        <v>284</v>
       </c>
       <c r="H94" s="28" t="s">
-        <v>229</v>
+        <v>285</v>
       </c>
       <c r="I94" s="29" t="s">
         <v>264</v>
@@ -6008,7 +6021,7 @@
         <v>2</v>
       </c>
       <c r="M94" s="29" t="s">
-        <v>2</v>
+        <v>127</v>
       </c>
       <c r="N94" s="29" t="s">
         <v>54</v>

</xml_diff>